<commit_message>
I've got an idea
</commit_message>
<xml_diff>
--- a/speaking.xlsx
+++ b/speaking.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId4"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="310" count="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="302" count="302">
   <si>
     <t>Timestamp</t>
   </si>
@@ -929,30 +929,6 @@
   </si>
   <si>
     <t>Be able to have the courage to speak.</t>
-  </si>
-  <si>
-    <t>A-C</t>
-  </si>
-  <si>
-    <t>ABC</t>
-  </si>
-  <si>
-    <t>AB-</t>
-  </si>
-  <si>
-    <t>---</t>
-  </si>
-  <si>
-    <t>-BC</t>
-  </si>
-  <si>
-    <t>A--</t>
-  </si>
-  <si>
-    <t>--C</t>
-  </si>
-  <si>
-    <t>-B-</t>
   </si>
 </sst>
 </file>
@@ -1320,7 +1296,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
   <dimension ref="A1:CJ40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -12019,10 +11995,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
-  <dimension ref="B1:AN25"/>
+  <dimension ref="A3:A25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.7109375" defaultRowHeight="12.75"/>
@@ -12030,3048 +12006,119 @@
     <col min="1" max="1" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:40" customFormat="false">
-      <c r="B1" s="0" t="str">
-        <v>aaron.nesnow846@gaston.k12.nc.us</v>
-      </c>
-      <c r="C1" s="0" t="str">
-        <v>adison.costner856@gaston.k12.nc.us</v>
-      </c>
-      <c r="D1" s="0" t="str">
-        <v>alana.williams574@gaston.k12.nc.us</v>
-      </c>
-      <c r="E1" s="0" t="str">
-        <v>alanie.odell901@gaston.k12.nc.us</v>
-      </c>
-      <c r="F1" s="0" t="str">
-        <v>aleigha.letterman215@gaston.k12.nc.us</v>
-      </c>
-      <c r="G1" s="0" t="str">
-        <v>aleigha.letterman215@gaston.k12.nc.us</v>
-      </c>
-      <c r="H1" s="0" t="str">
-        <v>anna.kleffnerspencer042@gaston.k12.nc.us</v>
-      </c>
-      <c r="I1" s="0" t="str">
-        <v>caleb.costner942@gaston.k12.nc.us</v>
-      </c>
-      <c r="J1" s="0" t="str">
-        <v>dalton.harmon921@gaston.k12.nc.us</v>
-      </c>
-      <c r="K1" s="0" t="str">
-        <v>douglas.farley537@gaston.k12.nc.us</v>
-      </c>
-      <c r="L1" s="0" t="str">
-        <v>elizabeth.suarez717@gaston.k12.nc.us</v>
-      </c>
-      <c r="M1" s="0" t="str">
-        <v>grace.deaton440@gaston.k12.nc.us</v>
-      </c>
-      <c r="N1" s="0" t="str">
-        <v>hannah.berckman208@gaston.k12.nc.us</v>
-      </c>
-      <c r="O1" s="0" t="str">
-        <v>hannah.cribby469@gaston.k12.nc.us</v>
-      </c>
-      <c r="P1" s="0" t="str">
-        <v>haylee.franckewitz955@gaston.k12.nc.us</v>
-      </c>
-      <c r="Q1" s="0" t="str">
-        <v>james.abee815@gaston.k12.nc.us</v>
-      </c>
-      <c r="R1" s="0" t="str">
-        <v>james.abee815@gaston.k12.nc.us</v>
-      </c>
-      <c r="S1" s="0" t="str">
-        <v>james.lynn958@gaston.k12.nc.us</v>
-      </c>
-      <c r="T1" s="0" t="str">
-        <v>jared.godwin616@gaston.k12.nc.us</v>
-      </c>
-      <c r="U1" s="0" t="str">
-        <v>jessica.kirby006@gaston.k12.nc.us</v>
-      </c>
-      <c r="V1" s="0" t="str">
-        <v>jessica.payne425@gaston.k12.nc.us</v>
-      </c>
-      <c r="W1" s="0" t="str">
-        <v>kalynne.helms096@gaston.k12.nc.us</v>
-      </c>
-      <c r="X1" s="0" t="str">
-        <v>karmen.scruggs776@gaston.k12.nc.us</v>
-      </c>
-      <c r="Y1" s="0" t="str">
-        <v>kayla.shannon027@gaston.k12.nc.us</v>
-      </c>
-      <c r="Z1" s="0" t="str">
-        <v>kayla.williamson843@gaston.k12.nc.us</v>
-      </c>
-      <c r="AA1" s="0" t="str">
-        <v>kimberly.queen686@gaston.k12.nc.us</v>
-      </c>
-      <c r="AB1" s="0" t="str">
-        <v>kyra.rhyne012@gaston.k12.nc.us</v>
-      </c>
-      <c r="AC1" s="0" t="str">
-        <v>kyra.rhyne012@gaston.k12.nc.us</v>
-      </c>
-      <c r="AD1" s="0" t="str">
-        <v>laurie.ricardo512@gaston.k12.nc.us</v>
-      </c>
-      <c r="AE1" s="0" t="str">
-        <v>ling.zhang885@gaston.k12.nc.us</v>
-      </c>
-      <c r="AF1" s="0" t="str">
-        <v>noah.wollin244@gaston.k12.nc.us</v>
-      </c>
-      <c r="AG1" s="0" t="str">
-        <v>olyvia.knight064@gaston.k12.nc.us</v>
-      </c>
-      <c r="AH1" s="0" t="str">
-        <v>parth.patel358@gaston.k12.nc.us</v>
-      </c>
-      <c r="AI1" s="0" t="str">
-        <v>piper.colangelo050@gaston.k12.nc.us</v>
-      </c>
-      <c r="AJ1" s="0" t="str">
-        <v>riley.kiefer729@gaston.k12.nc.us</v>
-      </c>
-      <c r="AK1" s="0" t="str">
-        <v>sarah.macon201@gaston.k12.nc.us</v>
-      </c>
-      <c r="AL1" s="0" t="str">
-        <v>scott.johnson192@gaston.k12.nc.us</v>
-      </c>
-      <c r="AM1" s="0" t="str">
-        <v>tiffany.weresow255@gaston.k12.nc.us</v>
-      </c>
-      <c r="AN1" s="0" t="str">
-        <v>weston.peavy213@gaston.k12.nc.us</v>
-      </c>
-    </row>
-    <row r="2" spans="2:40" customFormat="false">
-      <c r="B2" s="0" t="str">
-        <v>Spanish II 1st</v>
-      </c>
-      <c r="C2" s="0" t="str">
-        <v>Spanish II 4th</v>
-      </c>
-      <c r="D2" s="0" t="str">
-        <v>Spanish II 4th</v>
-      </c>
-      <c r="E2" s="0" t="str">
-        <v>Spanish II 4th</v>
-      </c>
-      <c r="F2" s="0" t="str">
-        <v>Spanish II 4th</v>
-      </c>
-      <c r="G2" s="0" t="str">
-        <v>Spanish II 4th</v>
-      </c>
-      <c r="H2" s="0" t="str">
-        <v>Spanish II 1st</v>
-      </c>
-      <c r="I2" s="0" t="str">
-        <v>Spanish II 1st</v>
-      </c>
-      <c r="J2" s="0" t="str">
-        <v>Spanish II 4th</v>
-      </c>
-      <c r="K2" s="0" t="str">
-        <v>Spanish II 1st</v>
-      </c>
-      <c r="L2" s="0" t="str">
-        <v>Spanish II 4th</v>
-      </c>
-      <c r="M2" s="0" t="str">
-        <v>Spanish II 4th</v>
-      </c>
-      <c r="N2" s="0" t="str">
-        <v>Spanish II 4th</v>
-      </c>
-      <c r="O2" s="0" t="str">
-        <v>Spanish II 1st</v>
-      </c>
-      <c r="P2" s="0" t="str">
-        <v>Spanish II 1st</v>
-      </c>
-      <c r="Q2" s="0" t="str">
-        <v>Spanish II 1st</v>
-      </c>
-      <c r="R2" s="0" t="str">
-        <v>Spanish II 1st</v>
-      </c>
-      <c r="S2" s="0" t="str">
-        <v>Spanish II 1st</v>
-      </c>
-      <c r="T2" s="0" t="str">
-        <v>Spanish II 1st</v>
-      </c>
-      <c r="U2" s="0" t="str">
-        <v>Spanish II 1st</v>
-      </c>
-      <c r="V2" s="0" t="str">
-        <v>Spanish II 1st</v>
-      </c>
-      <c r="W2" s="0" t="str">
-        <v>Spanish II 4th</v>
-      </c>
-      <c r="X2" s="0" t="str">
-        <v>Spanish II 4th</v>
-      </c>
-      <c r="Y2" s="0" t="str">
-        <v>Spanish II 1st</v>
-      </c>
-      <c r="Z2" s="0" t="str">
-        <v>Spanish II 1st</v>
-      </c>
-      <c r="AA2" s="0" t="str">
-        <v>Spanish II 1st</v>
-      </c>
-      <c r="AB2" s="0" t="str">
-        <v>Spanish II 4th</v>
-      </c>
-      <c r="AC2" s="0" t="str">
-        <v>Spanish II 4th</v>
-      </c>
-      <c r="AD2" s="0" t="str">
-        <v>Spanish II 1st</v>
-      </c>
-      <c r="AE2" s="0" t="str">
-        <v>Spanish II 4th</v>
-      </c>
-      <c r="AF2" s="0" t="str">
-        <v>Spanish II 1st</v>
-      </c>
-      <c r="AG2" s="0" t="str">
-        <v>Spanish II 4th</v>
-      </c>
-      <c r="AH2" s="0" t="str">
-        <v>Spanish II 1st</v>
-      </c>
-      <c r="AI2" s="0" t="str">
-        <v>Spanish II 1st</v>
-      </c>
-      <c r="AJ2" s="0" t="str">
-        <v>Spanish II 4th</v>
-      </c>
-      <c r="AK2" s="0" t="str">
-        <v>Spanish II 1st</v>
-      </c>
-      <c r="AL2" s="0" t="str">
-        <v>Spanish II 1st</v>
-      </c>
-      <c r="AM2" s="0" t="str">
-        <v>Spanish II 1st</v>
-      </c>
-      <c r="AN2" s="0" t="str">
-        <v>Spanish II 4th</v>
-      </c>
-    </row>
-    <row r="3" spans="1:40" customFormat="false">
+    <row r="3" spans="1:1" customFormat="false">
       <c r="A3" s="0" t="str">
         <v>NOVICE ask/respond to  predictable, formulaic questions</v>
       </c>
-      <c r="B3" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="C3" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="D3" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="E3" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="F3" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="G3" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="H3" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="I3" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="J3" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="K3" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="L3" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="M3" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="N3" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="O3" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="P3" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="Q3" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="R3" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="S3" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="T3" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="U3" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="V3" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="W3" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="X3" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="Y3" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="Z3" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="AA3" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AB3" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="AC3" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="AD3" s="0" t="str">
-        <v>-B-</v>
-      </c>
-      <c r="AE3" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AF3" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AG3" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AH3" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AI3" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AJ3" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AK3" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="AL3" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AM3" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="AN3" s="0" t="str">
-        <v>A--</v>
-      </c>
     </row>
-    <row r="4" spans="1:40" customFormat="false">
+    <row r="4" spans="1:1" customFormat="false">
       <c r="A4" s="0" t="str">
         <v>NOVICE list, name, identify</v>
       </c>
-      <c r="B4" s="0" t="str">
-        <v>-B-</v>
-      </c>
-      <c r="C4" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="D4" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="E4" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="F4" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="G4" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="H4" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="I4" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="J4" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="K4" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="L4" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="M4" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="N4" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="O4" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="P4" s="0" t="str">
-        <v>-B-</v>
-      </c>
-      <c r="Q4" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="R4" s="0" t="str">
-        <v>-B-</v>
-      </c>
-      <c r="S4" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="T4" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="U4" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="V4" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="W4" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="X4" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="Y4" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="Z4" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="AA4" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="AB4" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="AC4" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AD4" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AE4" s="0" t="str">
-        <v>-B-</v>
-      </c>
-      <c r="AF4" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AG4" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AH4" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="AI4" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="AJ4" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="AK4" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="AL4" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="AM4" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="AN4" s="0" t="str">
-        <v>---</v>
-      </c>
     </row>
-    <row r="5" spans="1:40" customFormat="false">
+    <row r="5" spans="1:1" customFormat="false">
       <c r="A5" s="0" t="str">
         <v>INTERMEDIATE ask, answer variety of questions</v>
       </c>
-      <c r="B5" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="C5" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="D5" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="E5" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="F5" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="G5" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="H5" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="I5" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="J5" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="K5" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="L5" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="M5" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="N5" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="O5" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="P5" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="Q5" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="R5" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="S5" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="T5" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="U5" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="V5" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="W5" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="X5" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="Y5" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="Z5" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="AA5" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AB5" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AC5" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AD5" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AE5" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="AF5" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AG5" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="AH5" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AI5" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AJ5" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AK5" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="AL5" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AM5" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="AN5" s="0" t="str">
-        <v>AB-</v>
-      </c>
     </row>
-    <row r="6" spans="1:40" customFormat="false">
+    <row r="6" spans="1:1" customFormat="false">
       <c r="A6" s="0" t="str">
         <v>INTERMEDIATE initiate, maintain, end conversation for basic needs/transactions</v>
       </c>
-      <c r="B6" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="C6" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="D6" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="E6" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="F6" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="G6" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="H6" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="I6" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="J6" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="K6" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="L6" s="0" t="str">
-        <v>-B-</v>
-      </c>
-      <c r="M6" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="N6" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="O6" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="P6" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="Q6" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="R6" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="S6" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="T6" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="U6" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="V6" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="W6" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="X6" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="Y6" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="Z6" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="AA6" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AB6" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AC6" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AD6" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AE6" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AF6" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AG6" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="AH6" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="AI6" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="AJ6" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AK6" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AL6" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="AM6" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AN6" s="0" t="str">
-        <v>-B-</v>
-      </c>
     </row>
-    <row r="7" spans="1:40" customFormat="false">
+    <row r="7" spans="1:1" customFormat="false">
       <c r="A7" s="0" t="str">
         <v>INTERMEDIATE communicate beyond "here &amp; now</v>
       </c>
-      <c r="B7" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="C7" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="D7" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="E7" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="F7" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="G7" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="H7" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="I7" s="0" t="str">
-        <v>-B-</v>
-      </c>
-      <c r="J7" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="K7" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="L7" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="M7" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="N7" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="O7" s="0" t="str">
-        <v>-B-</v>
-      </c>
-      <c r="P7" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="Q7" s="0" t="str">
-        <v>-B-</v>
-      </c>
-      <c r="R7" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="S7" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="T7" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="U7" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="V7" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="W7" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="X7" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="Y7" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="Z7" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AA7" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AB7" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="AC7" s="0" t="str">
-        <v>-B-</v>
-      </c>
-      <c r="AD7" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="AE7" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AF7" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AG7" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AH7" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="AI7" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AJ7" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AK7" s="0" t="str">
-        <v>-B-</v>
-      </c>
-      <c r="AL7" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="AM7" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="AN7" s="0" t="str">
-        <v>---</v>
-      </c>
     </row>
-    <row r="8" spans="1:40" customFormat="false">
+    <row r="8" spans="1:1" customFormat="false">
       <c r="A8" s="0" t="str">
         <v>NOVICE practiced words, phrases, sentences</v>
       </c>
-      <c r="B8" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="C8" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="D8" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="E8" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="F8" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="G8" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="H8" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="I8" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="J8" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="K8" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="L8" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="M8" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="N8" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="O8" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="P8" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="Q8" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="R8" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="S8" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="T8" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="U8" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="V8" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="W8" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="X8" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="Y8" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="Z8" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AA8" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AB8" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AC8" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AD8" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="AE8" s="0" t="str">
-        <v>-B-</v>
-      </c>
-      <c r="AF8" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AG8" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AH8" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AI8" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AJ8" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AK8" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="AL8" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AM8" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="AN8" s="0" t="str">
-        <v>AB-</v>
-      </c>
     </row>
-    <row r="9" spans="1:40" customFormat="false">
+    <row r="9" spans="1:1" customFormat="false">
       <c r="A9" s="0" t="str">
         <v>NOVICE formulaic/memorized questions</v>
       </c>
-      <c r="B9" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="C9" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="D9" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="E9" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="F9" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="G9" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="H9" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="I9" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="J9" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="K9" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="L9" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="M9" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="N9" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="O9" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="P9" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="Q9" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="R9" s="0" t="str">
-        <v>-B-</v>
-      </c>
-      <c r="S9" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="T9" s="0" t="str">
-        <v>-B-</v>
-      </c>
-      <c r="U9" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="V9" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="W9" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="X9" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="Y9" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="Z9" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AA9" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="AB9" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="AC9" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AD9" s="0" t="str">
-        <v>-B-</v>
-      </c>
-      <c r="AE9" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="AF9" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AG9" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AH9" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="AI9" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AJ9" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AK9" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="AL9" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="AM9" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="AN9" s="0" t="str">
-        <v>---</v>
-      </c>
     </row>
-    <row r="10" spans="1:40" customFormat="false">
+    <row r="10" spans="1:1" customFormat="false">
       <c r="A10" s="0" t="str">
         <v>INTERMEDIATE strings of sentences</v>
       </c>
-      <c r="B10" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="C10" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="D10" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="E10" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="F10" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="G10" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="H10" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="I10" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="J10" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="K10" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="L10" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="M10" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="N10" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="O10" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="P10" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="Q10" s="0" t="str">
-        <v>-B-</v>
-      </c>
-      <c r="R10" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="S10" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="T10" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="U10" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="V10" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="W10" s="0" t="str">
-        <v>-B-</v>
-      </c>
-      <c r="X10" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="Y10" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="Z10" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="AA10" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AB10" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AC10" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AD10" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AE10" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AF10" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="AG10" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AH10" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AI10" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AJ10" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AK10" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="AL10" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="AM10" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AN10" s="0" t="str">
-        <v>-B-</v>
-      </c>
     </row>
-    <row r="11" spans="1:40" customFormat="false">
+    <row r="11" spans="1:1" customFormat="false">
       <c r="A11" s="0" t="str">
         <v>INTERMEDIATE connected sentences</v>
       </c>
-      <c r="B11" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="C11" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="D11" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="E11" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="F11" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="G11" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="H11" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="I11" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="J11" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="K11" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="L11" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="M11" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="N11" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="O11" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="P11" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="Q11" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="R11" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="S11" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="T11" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="U11" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="V11" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="W11" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="X11" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="Y11" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="Z11" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="AA11" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AB11" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AC11" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="AD11" s="0" t="str">
-        <v>-B-</v>
-      </c>
-      <c r="AE11" s="0" t="str">
-        <v>-B-</v>
-      </c>
-      <c r="AF11" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AG11" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="AH11" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AI11" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AJ11" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AK11" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="AL11" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="AM11" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AN11" s="0" t="str">
-        <v>-B-</v>
-      </c>
     </row>
-    <row r="12" spans="1:40" customFormat="false">
+    <row r="12" spans="1:1" customFormat="false">
       <c r="A12" s="0" t="str">
         <v>INTERMEDIATE ask questions to initiate/ sustain conversation</v>
       </c>
-      <c r="B12" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="C12" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="D12" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="E12" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="F12" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="G12" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="H12" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="I12" s="0" t="str">
-        <v>-B-</v>
-      </c>
-      <c r="J12" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="K12" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="L12" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="M12" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="N12" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="O12" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="P12" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="Q12" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="R12" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="S12" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="T12" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="U12" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="V12" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="W12" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="X12" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="Y12" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="Z12" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="AA12" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AB12" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AC12" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AD12" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AE12" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="AF12" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="AG12" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="AH12" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AI12" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AJ12" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AK12" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AL12" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AM12" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="AN12" s="0" t="str">
-        <v>A--</v>
-      </c>
     </row>
-    <row r="13" spans="1:40" customFormat="false">
+    <row r="13" spans="1:1" customFormat="false">
       <c r="A13" s="0" t="str">
         <v>NOVICE high-frequency</v>
       </c>
-      <c r="B13" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="C13" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="D13" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="E13" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="F13" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="G13" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="H13" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="I13" s="0" t="str">
-        <v>-B-</v>
-      </c>
-      <c r="J13" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="K13" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="L13" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="M13" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="N13" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="O13" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="P13" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="Q13" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="R13" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="S13" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="T13" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="U13" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="V13" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="W13" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="X13" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="Y13" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="Z13" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AA13" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AB13" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="AC13" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AD13" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AE13" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AF13" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AG13" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AH13" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AI13" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AJ13" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="AK13" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AL13" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="AM13" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="AN13" s="0" t="str">
-        <v>---</v>
-      </c>
     </row>
-    <row r="14" spans="1:40" customFormat="false">
+    <row r="14" spans="1:1" customFormat="false">
       <c r="A14" s="0" t="str">
         <v>NOVICE formulaic</v>
       </c>
-      <c r="B14" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="C14" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="D14" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="E14" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="F14" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="G14" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="H14" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="I14" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="J14" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="K14" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="L14" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="M14" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="N14" s="0" t="str">
-        <v>-B-</v>
-      </c>
-      <c r="O14" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="P14" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="Q14" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="R14" s="0" t="str">
-        <v>-B-</v>
-      </c>
-      <c r="S14" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="T14" s="0" t="str">
-        <v>-B-</v>
-      </c>
-      <c r="U14" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="V14" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="W14" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="X14" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="Y14" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="Z14" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="AA14" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AB14" s="0" t="str">
-        <v>-B-</v>
-      </c>
-      <c r="AC14" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AD14" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AE14" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="AF14" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AG14" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AH14" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="AI14" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="AJ14" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AK14" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AL14" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="AM14" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AN14" s="0" t="str">
-        <v>---</v>
-      </c>
     </row>
-    <row r="15" spans="1:40" customFormat="false">
+    <row r="15" spans="1:1" customFormat="false">
       <c r="A15" s="0" t="str">
         <v>NOVICE practiced</v>
       </c>
-      <c r="B15" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="C15" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="D15" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="E15" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="F15" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="G15" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="H15" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="I15" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="J15" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="K15" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="L15" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="M15" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="N15" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="O15" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="P15" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="Q15" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="R15" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="S15" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="T15" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="U15" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="V15" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="W15" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="X15" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="Y15" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="Z15" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AA15" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AB15" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AC15" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AD15" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="AE15" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AF15" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AG15" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AH15" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AI15" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="AJ15" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AK15" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="AL15" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="AM15" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="AN15" s="0" t="str">
-        <v>AB-</v>
-      </c>
     </row>
-    <row r="16" spans="1:40" customFormat="false">
+    <row r="16" spans="1:1" customFormat="false">
       <c r="A16" s="0" t="str">
         <v>INTERMEDIATE familiar themes/topics</v>
       </c>
-      <c r="B16" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="C16" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="D16" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="E16" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="F16" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="G16" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="H16" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="I16" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="J16" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="K16" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="L16" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="M16" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="N16" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="O16" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="P16" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="Q16" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="R16" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="S16" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="T16" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="U16" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="V16" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="W16" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="X16" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="Y16" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="Z16" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AA16" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AB16" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AC16" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AD16" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="AE16" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AF16" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AG16" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AH16" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AI16" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AJ16" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="AK16" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="AL16" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="AM16" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AN16" s="0" t="str">
-        <v>AB-</v>
-      </c>
     </row>
-    <row r="17" spans="1:40" customFormat="false">
+    <row r="17" spans="1:1" customFormat="false">
       <c r="A17" s="0" t="str">
         <v>INTERMEDIATE personalized</v>
       </c>
-      <c r="B17" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="C17" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="D17" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="E17" s="0" t="str">
-        <v>-B-</v>
-      </c>
-      <c r="F17" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="G17" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="H17" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="I17" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="J17" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="K17" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="L17" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="M17" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="N17" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="O17" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="P17" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="Q17" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="R17" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="S17" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="T17" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="U17" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="V17" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="W17" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="X17" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="Y17" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="Z17" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="AA17" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AB17" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AC17" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AD17" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AE17" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AF17" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AG17" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="AH17" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AI17" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="AJ17" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AK17" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AL17" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AM17" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AN17" s="0" t="str">
-        <v>---</v>
-      </c>
     </row>
-    <row r="18" spans="1:40" customFormat="false">
+    <row r="18" spans="1:1" customFormat="false">
       <c r="A18" s="0" t="str">
         <v>NOVICE imitate modeled words</v>
       </c>
-      <c r="B18" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="C18" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="D18" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="E18" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="F18" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="G18" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="H18" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="I18" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="J18" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="K18" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="L18" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="M18" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="N18" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="O18" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="P18" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="Q18" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="R18" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="S18" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="T18" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="U18" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="V18" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="W18" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="X18" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="Y18" s="0" t="str">
-        <v>-B-</v>
-      </c>
-      <c r="Z18" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AA18" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="AB18" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AC18" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AD18" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="AE18" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AF18" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AG18" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AH18" s="0" t="str">
-        <v>-B-</v>
-      </c>
-      <c r="AI18" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="AJ18" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AK18" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="AL18" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="AM18" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="AN18" s="0" t="str">
-        <v>-B-</v>
-      </c>
     </row>
-    <row r="19" spans="1:40" customFormat="false">
+    <row r="19" spans="1:1" customFormat="false">
       <c r="A19" s="0" t="str">
         <v>NOVICE use facial expressions, gestures</v>
       </c>
-      <c r="B19" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="C19" s="0" t="str">
-        <v>-B-</v>
-      </c>
-      <c r="D19" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="E19" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="F19" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="G19" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="H19" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="I19" s="0" t="str">
-        <v>-B-</v>
-      </c>
-      <c r="J19" s="0" t="str">
-        <v>-B-</v>
-      </c>
-      <c r="K19" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="L19" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="M19" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="N19" s="0" t="str">
-        <v>-B-</v>
-      </c>
-      <c r="O19" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="P19" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="Q19" s="0" t="str">
-        <v>-B-</v>
-      </c>
-      <c r="R19" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="S19" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="T19" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="U19" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="V19" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="W19" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="X19" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="Y19" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="Z19" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AA19" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="AB19" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AC19" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AD19" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AE19" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="AF19" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="AG19" s="0" t="str">
-        <v>-B-</v>
-      </c>
-      <c r="AH19" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="AI19" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AJ19" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="AK19" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AL19" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="AM19" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AN19" s="0" t="str">
-        <v>---</v>
-      </c>
     </row>
-    <row r="20" spans="1:40" customFormat="false">
+    <row r="20" spans="1:1" customFormat="false">
       <c r="A20" s="0" t="str">
         <v>NOVICE resort to first language</v>
       </c>
-      <c r="B20" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="C20" s="0" t="str">
-        <v>-B-</v>
-      </c>
-      <c r="D20" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="E20" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="F20" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="G20" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="H20" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="I20" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="J20" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="K20" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="L20" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="M20" s="0" t="str">
-        <v>-B-</v>
-      </c>
-      <c r="N20" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="O20" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="P20" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="Q20" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="R20" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="S20" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="T20" s="0" t="str">
-        <v>-B-</v>
-      </c>
-      <c r="U20" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="V20" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="W20" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="X20" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="Y20" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="Z20" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AA20" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AB20" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AC20" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AD20" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AE20" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AF20" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AG20" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AH20" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AI20" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AJ20" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AK20" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AL20" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AM20" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AN20" s="0" t="str">
-        <v>AB-</v>
-      </c>
     </row>
-    <row r="21" spans="1:40" customFormat="false">
+    <row r="21" spans="1:1" customFormat="false">
       <c r="A21" s="0" t="str">
         <v>NOVICE repeat/request repetition</v>
       </c>
-      <c r="B21" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="C21" s="0" t="str">
-        <v>-B-</v>
-      </c>
-      <c r="D21" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="E21" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="F21" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="G21" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="H21" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="I21" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="J21" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="K21" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="L21" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="M21" s="0" t="str">
-        <v>-B-</v>
-      </c>
-      <c r="N21" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="O21" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="P21" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="Q21" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="R21" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="S21" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="T21" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="U21" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="V21" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="W21" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="X21" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="Y21" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="Z21" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AA21" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AB21" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AC21" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="AD21" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AE21" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AF21" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="AG21" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AH21" s="0" t="str">
-        <v>-B-</v>
-      </c>
-      <c r="AI21" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AJ21" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AK21" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AL21" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="AM21" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AN21" s="0" t="str">
-        <v>-B-</v>
-      </c>
     </row>
-    <row r="22" spans="1:40" customFormat="false">
+    <row r="22" spans="1:1" customFormat="false">
       <c r="A22" s="0" t="str">
         <v>NOVICE indicate lack of understanding</v>
       </c>
-      <c r="B22" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="C22" s="0" t="str">
-        <v>-B-</v>
-      </c>
-      <c r="D22" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="E22" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="F22" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="G22" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="H22" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="I22" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="J22" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="K22" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="L22" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="M22" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="N22" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="O22" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="P22" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="Q22" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="R22" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="S22" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="T22" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="U22" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="V22" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="W22" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="X22" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="Y22" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="Z22" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AA22" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AB22" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AC22" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AD22" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AE22" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AF22" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="AG22" s="0" t="str">
-        <v>-B-</v>
-      </c>
-      <c r="AH22" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AI22" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AJ22" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AK22" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AL22" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AM22" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AN22" s="0" t="str">
-        <v>---</v>
-      </c>
     </row>
-    <row r="23" spans="1:40" customFormat="false">
+    <row r="23" spans="1:1" customFormat="false">
       <c r="A23" s="0" t="str">
         <v>INTERMEDIATE ask questions, request clarification</v>
       </c>
-      <c r="B23" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="C23" s="0" t="str">
-        <v>-B-</v>
-      </c>
-      <c r="D23" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="E23" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="F23" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="G23" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="H23" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="I23" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="J23" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="K23" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="L23" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="M23" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="N23" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="O23" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="P23" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="Q23" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="R23" s="0" t="str">
-        <v>-B-</v>
-      </c>
-      <c r="S23" s="0" t="str">
-        <v>-B-</v>
-      </c>
-      <c r="T23" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="U23" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="V23" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="W23" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="X23" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="Y23" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="Z23" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="AA23" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AB23" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AC23" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AD23" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="AE23" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AF23" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AG23" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="AH23" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="AI23" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AJ23" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AK23" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="AL23" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="AM23" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="AN23" s="0" t="str">
-        <v>---</v>
-      </c>
     </row>
-    <row r="24" spans="1:40" customFormat="false">
+    <row r="24" spans="1:1" customFormat="false">
       <c r="A24" s="0" t="str">
         <v>INTERMEDIATE self-correct or restate when not understood</v>
       </c>
-      <c r="B24" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="C24" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="D24" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="E24" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="F24" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="G24" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="H24" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="I24" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="J24" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="K24" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="L24" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="M24" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="N24" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="O24" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="P24" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="Q24" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="R24" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="S24" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="T24" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="U24" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="V24" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="W24" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="X24" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="Y24" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="Z24" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AA24" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="AB24" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="AC24" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="AD24" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="AE24" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AF24" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AG24" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AH24" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AI24" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AJ24" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AK24" s="0" t="str">
-        <v>A--</v>
-      </c>
-      <c r="AL24" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="AM24" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AN24" s="0" t="str">
-        <v>-B-</v>
-      </c>
     </row>
-    <row r="25" spans="1:40" customFormat="false">
+    <row r="25" spans="1:1" customFormat="false">
       <c r="A25" s="0" t="str">
         <v>INTERMEDIATE circumlocute</v>
-      </c>
-      <c r="B25" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="C25" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="D25" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="E25" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="F25" s="0" t="str">
-        <v>A-C</v>
-      </c>
-      <c r="G25" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="H25" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="I25" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="J25" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="K25" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="L25" s="0" t="str">
-        <v>-B-</v>
-      </c>
-      <c r="M25" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="N25" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="O25" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="P25" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="Q25" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="R25" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="S25" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="T25" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="U25" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="V25" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="W25" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="X25" s="0" t="str">
-        <v>-B-</v>
-      </c>
-      <c r="Y25" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="Z25" s="0" t="str">
-        <v>--C</v>
-      </c>
-      <c r="AA25" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AB25" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AC25" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AD25" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AE25" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AF25" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="AG25" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AH25" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AI25" s="0" t="str">
-        <v>---</v>
-      </c>
-      <c r="AJ25" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AK25" s="0" t="str">
-        <v>ABC</v>
-      </c>
-      <c r="AL25" s="0" t="str">
-        <v>-BC</v>
-      </c>
-      <c r="AM25" s="0" t="str">
-        <v>AB-</v>
-      </c>
-      <c r="AN25" s="0" t="str">
-        <v>---</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleaned up a lot of code
</commit_message>
<xml_diff>
--- a/speaking.xlsx
+++ b/speaking.xlsx
@@ -11995,130 +11995,3179 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
-  <dimension ref="A3:A25"/>
+  <dimension ref="B1:AN26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="F21" sqref="A1:AN27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.7109375" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="27.5703125" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:1" customFormat="false">
-      <c r="A3" s="0" t="str">
+    <row r="1" spans="2:40" customFormat="false">
+      <c r="B1" s="0" t="str">
+        <v>aaron.nesnow846@gaston.k12.nc.us</v>
+      </c>
+      <c r="C1" s="0" t="str">
+        <v>adison.costner856@gaston.k12.nc.us</v>
+      </c>
+      <c r="D1" s="0" t="str">
+        <v>alana.williams574@gaston.k12.nc.us</v>
+      </c>
+      <c r="E1" s="0" t="str">
+        <v>alanie.odell901@gaston.k12.nc.us</v>
+      </c>
+      <c r="F1" s="0" t="str">
+        <v>aleigha.letterman215@gaston.k12.nc.us</v>
+      </c>
+      <c r="G1" s="0" t="str">
+        <v>aleigha.letterman215@gaston.k12.nc.us</v>
+      </c>
+      <c r="H1" s="0" t="str">
+        <v>anna.kleffnerspencer042@gaston.k12.nc.us</v>
+      </c>
+      <c r="I1" s="0" t="str">
+        <v>caleb.costner942@gaston.k12.nc.us</v>
+      </c>
+      <c r="J1" s="0" t="str">
+        <v>dalton.harmon921@gaston.k12.nc.us</v>
+      </c>
+      <c r="K1" s="0" t="str">
+        <v>douglas.farley537@gaston.k12.nc.us</v>
+      </c>
+      <c r="L1" s="0" t="str">
+        <v>elizabeth.suarez717@gaston.k12.nc.us</v>
+      </c>
+      <c r="M1" s="0" t="str">
+        <v>grace.deaton440@gaston.k12.nc.us</v>
+      </c>
+      <c r="N1" s="0" t="str">
+        <v>hannah.berckman208@gaston.k12.nc.us</v>
+      </c>
+      <c r="O1" s="0" t="str">
+        <v>hannah.cribby469@gaston.k12.nc.us</v>
+      </c>
+      <c r="P1" s="0" t="str">
+        <v>haylee.franckewitz955@gaston.k12.nc.us</v>
+      </c>
+      <c r="Q1" s="0" t="str">
+        <v>james.abee815@gaston.k12.nc.us</v>
+      </c>
+      <c r="R1" s="0" t="str">
+        <v>james.abee815@gaston.k12.nc.us</v>
+      </c>
+      <c r="S1" s="0" t="str">
+        <v>james.lynn958@gaston.k12.nc.us</v>
+      </c>
+      <c r="T1" s="0" t="str">
+        <v>jared.godwin616@gaston.k12.nc.us</v>
+      </c>
+      <c r="U1" s="0" t="str">
+        <v>jessica.kirby006@gaston.k12.nc.us</v>
+      </c>
+      <c r="V1" s="0" t="str">
+        <v>jessica.payne425@gaston.k12.nc.us</v>
+      </c>
+      <c r="W1" s="0" t="str">
+        <v>kalynne.helms096@gaston.k12.nc.us</v>
+      </c>
+      <c r="X1" s="0" t="str">
+        <v>karmen.scruggs776@gaston.k12.nc.us</v>
+      </c>
+      <c r="Y1" s="0" t="str">
+        <v>kayla.shannon027@gaston.k12.nc.us</v>
+      </c>
+      <c r="Z1" s="0" t="str">
+        <v>kayla.williamson843@gaston.k12.nc.us</v>
+      </c>
+      <c r="AA1" s="0" t="str">
+        <v>kimberly.queen686@gaston.k12.nc.us</v>
+      </c>
+      <c r="AB1" s="0" t="str">
+        <v>kyra.rhyne012@gaston.k12.nc.us</v>
+      </c>
+      <c r="AC1" s="0" t="str">
+        <v>kyra.rhyne012@gaston.k12.nc.us</v>
+      </c>
+      <c r="AD1" s="0" t="str">
+        <v>laurie.ricardo512@gaston.k12.nc.us</v>
+      </c>
+      <c r="AE1" s="0" t="str">
+        <v>ling.zhang885@gaston.k12.nc.us</v>
+      </c>
+      <c r="AF1" s="0" t="str">
+        <v>noah.wollin244@gaston.k12.nc.us</v>
+      </c>
+      <c r="AG1" s="0" t="str">
+        <v>olyvia.knight064@gaston.k12.nc.us</v>
+      </c>
+      <c r="AH1" s="0" t="str">
+        <v>parth.patel358@gaston.k12.nc.us</v>
+      </c>
+      <c r="AI1" s="0" t="str">
+        <v>piper.colangelo050@gaston.k12.nc.us</v>
+      </c>
+      <c r="AJ1" s="0" t="str">
+        <v>riley.kiefer729@gaston.k12.nc.us</v>
+      </c>
+      <c r="AK1" s="0" t="str">
+        <v>sarah.macon201@gaston.k12.nc.us</v>
+      </c>
+      <c r="AL1" s="0" t="str">
+        <v>scott.johnson192@gaston.k12.nc.us</v>
+      </c>
+      <c r="AM1" s="0" t="str">
+        <v>tiffany.weresow255@gaston.k12.nc.us</v>
+      </c>
+      <c r="AN1" s="0" t="str">
+        <v>weston.peavy213@gaston.k12.nc.us</v>
+      </c>
+    </row>
+    <row r="2" spans="2:40" customFormat="false">
+      <c r="B2" s="0" t="str">
+        <v>http://gecaaronnespanol.blogspot.com/p/speaking.html</v>
+      </c>
+      <c r="C2" s="0" t="str">
+        <v>http://gecadisonsespanol.blogspot.com/p/speaking.html</v>
+      </c>
+      <c r="D2" s="0" t="str">
+        <v>http://gecalanawespanol.blogspot.com/p/speaking.html</v>
+      </c>
+      <c r="E2" s="0" t="str">
+        <v>http://gecalanieoespanol.blogspot.com/p/speaking.html</v>
+      </c>
+      <c r="F2" s="0" t="str">
+        <v>http://gecaleighalespanol.blogspot.com/</v>
+      </c>
+      <c r="G2" s="0" t="str">
+        <v>http://gecaleighalespanol.blogspot.com/p/speaking.html?_sm_au_=iRV4H734DJR712BH</v>
+      </c>
+      <c r="H2" s="0" t="str">
+        <v>http://gecannaks.blogspot.com/p/speaking.html</v>
+      </c>
+      <c r="I2" s="0" t="str">
+        <v>http://geccalebcespanol.blogspot.com/p/speaking.html</v>
+      </c>
+      <c r="J2" s="0" t="str">
+        <v>http://gecdaltonhespanol.blogspot.com/p/speaking.html</v>
+      </c>
+      <c r="K2" s="0" t="str">
+        <v>http://gecdouglasfespanol.blogspot.com/p/speaking.html</v>
+      </c>
+      <c r="L2" s="0" t="str">
+        <v>http://gecelizabethsespanol.blogspot.com/p/speaking.html</v>
+      </c>
+      <c r="M2" s="0" t="str">
+        <v>http://gecgracedespanol.blogspot.com/p/speaking.html</v>
+      </c>
+      <c r="N2" s="0" t="str">
+        <v>http://gechannahbespanol.blogspot.com/p/speaking.html</v>
+      </c>
+      <c r="O2" s="0" t="str">
+        <v>http://gechannahcespanol.blogspot.com/p/speaking.html</v>
+      </c>
+      <c r="P2" s="0" t="str">
+        <v>notebook</v>
+      </c>
+      <c r="Q2" s="0" t="str">
+        <v xml:space="preserve">http://gecloganaespanol.blogspot.com/p/speaking.html </v>
+      </c>
+      <c r="R2" s="0" t="str">
+        <v>http://gecloganaespanol.blogspot.com/p/speaking.html</v>
+      </c>
+      <c r="S2" s="0" t="str">
+        <v>http://gecjameslespanol.blogspot.com/p/speaking.html</v>
+      </c>
+      <c r="T2" s="0" t="str">
+        <v>Clavo: fue</v>
+      </c>
+      <c r="U2" s="0" t="str">
+        <v>http://gecjessicakespanol.blogspot.com/</v>
+      </c>
+      <c r="V2" s="0" t="str">
+        <v>http://gecjessicapespanol.blogspot.com/2017/02/hablar-portfolio.html</v>
+      </c>
+      <c r="W2" s="0" t="str">
+        <v>http://geckalynnehespanol.blogspot.com/p/speaking.html</v>
+      </c>
+      <c r="X2" s="0" t="str">
+        <v>http://geckarmensespanol.blogspot.com/p/speaking.html</v>
+      </c>
+      <c r="Y2" s="0" t="str">
+        <v>https://geckshannon.blogspot.com/b/post-preview?token=ujT-H1oBAAA.cBZXbAHzfkhewsrLBQwjCzCTaf9-aCxkbnLXCIU4J90SukY8Z8vcHzRZ8qg1eH2_dcqow_gOF0bmtMAVSuDZNQ.x5nCMzkXswb3fjHitapT9A&amp;postId=5070485297239961755&amp;type=PAGE</v>
+      </c>
+      <c r="Z2" s="0" t="str">
+        <v>http://geckaylawespanol.blogspot.com/p/speaking.html</v>
+      </c>
+      <c r="AA2" s="0" t="str">
+        <v>paper</v>
+      </c>
+      <c r="AB2" s="0" t="str">
+        <v>http://geckyrarespanol.blogspot.com/p/speaking.html</v>
+      </c>
+      <c r="AC2" s="0" t="str">
+        <v>http://geckyrarespanol.blogspot.com/p/speaking.html</v>
+      </c>
+      <c r="AD2" s="0" t="str">
+        <v>http://geclaurier.blogspot.com/p/speaking.html</v>
+      </c>
+      <c r="AE2" s="0" t="str">
+        <v>http://geclingespanol.blogspot.com/p/speaking.html</v>
+      </c>
+      <c r="AF2" s="0" t="str">
+        <v>http://gecnoahwespanol.blogspot.com/p/speaking.html</v>
+      </c>
+      <c r="AG2" s="0" t="str">
+        <v>http://gecolyviakespanol.blogspot.com/p/speaking.html</v>
+      </c>
+      <c r="AH2" s="0" t="str">
+        <v>http://gecparthespanol.blogspot.com/p/speaking.html</v>
+      </c>
+      <c r="AI2" s="0" t="str">
+        <v>http://gecpipercespanol.blogspot.com/p/speaking.html</v>
+      </c>
+      <c r="AJ2" s="0" t="str">
+        <v>https://gecrileykespanol.blogspot.com/p/speaking.html</v>
+      </c>
+      <c r="AK2" s="0" t="str">
+        <v>http://gecsarahmespanol.blogspot.com/p/speaking.html</v>
+      </c>
+      <c r="AL2" s="0" t="str">
+        <v>http://gecchristopherjespanol.blogspot.com/p/speaking.html</v>
+      </c>
+      <c r="AM2" s="0" t="str">
+        <v>http://gectiffanywespanol.blogspot.com/p/speaking.html</v>
+      </c>
+      <c r="AN2" s="0" t="str">
+        <v>http://gecwestonpespanol.blogspot.com/p/speaking.html</v>
+      </c>
+    </row>
+    <row r="3" spans="2:40" customFormat="false">
+      <c r="B3" s="0" t="str">
+        <v>Spanish II 1st</v>
+      </c>
+      <c r="C3" s="0" t="str">
+        <v>Spanish II 4th</v>
+      </c>
+      <c r="D3" s="0" t="str">
+        <v>Spanish II 4th</v>
+      </c>
+      <c r="E3" s="0" t="str">
+        <v>Spanish II 4th</v>
+      </c>
+      <c r="F3" s="0" t="str">
+        <v>Spanish II 4th</v>
+      </c>
+      <c r="G3" s="0" t="str">
+        <v>Spanish II 4th</v>
+      </c>
+      <c r="H3" s="0" t="str">
+        <v>Spanish II 1st</v>
+      </c>
+      <c r="I3" s="0" t="str">
+        <v>Spanish II 1st</v>
+      </c>
+      <c r="J3" s="0" t="str">
+        <v>Spanish II 4th</v>
+      </c>
+      <c r="K3" s="0" t="str">
+        <v>Spanish II 1st</v>
+      </c>
+      <c r="L3" s="0" t="str">
+        <v>Spanish II 4th</v>
+      </c>
+      <c r="M3" s="0" t="str">
+        <v>Spanish II 4th</v>
+      </c>
+      <c r="N3" s="0" t="str">
+        <v>Spanish II 4th</v>
+      </c>
+      <c r="O3" s="0" t="str">
+        <v>Spanish II 1st</v>
+      </c>
+      <c r="P3" s="0" t="str">
+        <v>Spanish II 1st</v>
+      </c>
+      <c r="Q3" s="0" t="str">
+        <v>Spanish II 1st</v>
+      </c>
+      <c r="R3" s="0" t="str">
+        <v>Spanish II 1st</v>
+      </c>
+      <c r="S3" s="0" t="str">
+        <v>Spanish II 1st</v>
+      </c>
+      <c r="T3" s="0" t="str">
+        <v>Spanish II 1st</v>
+      </c>
+      <c r="U3" s="0" t="str">
+        <v>Spanish II 1st</v>
+      </c>
+      <c r="V3" s="0" t="str">
+        <v>Spanish II 1st</v>
+      </c>
+      <c r="W3" s="0" t="str">
+        <v>Spanish II 4th</v>
+      </c>
+      <c r="X3" s="0" t="str">
+        <v>Spanish II 4th</v>
+      </c>
+      <c r="Y3" s="0" t="str">
+        <v>Spanish II 1st</v>
+      </c>
+      <c r="Z3" s="0" t="str">
+        <v>Spanish II 1st</v>
+      </c>
+      <c r="AA3" s="0" t="str">
+        <v>Spanish II 1st</v>
+      </c>
+      <c r="AB3" s="0" t="str">
+        <v>Spanish II 4th</v>
+      </c>
+      <c r="AC3" s="0" t="str">
+        <v>Spanish II 4th</v>
+      </c>
+      <c r="AD3" s="0" t="str">
+        <v>Spanish II 1st</v>
+      </c>
+      <c r="AE3" s="0" t="str">
+        <v>Spanish II 4th</v>
+      </c>
+      <c r="AF3" s="0" t="str">
+        <v>Spanish II 1st</v>
+      </c>
+      <c r="AG3" s="0" t="str">
+        <v>Spanish II 4th</v>
+      </c>
+      <c r="AH3" s="0" t="str">
+        <v>Spanish II 1st</v>
+      </c>
+      <c r="AI3" s="0" t="str">
+        <v>Spanish II 1st</v>
+      </c>
+      <c r="AJ3" s="0" t="str">
+        <v>Spanish II 4th</v>
+      </c>
+      <c r="AK3" s="0" t="str">
+        <v>Spanish II 1st</v>
+      </c>
+      <c r="AL3" s="0" t="str">
+        <v>Spanish II 1st</v>
+      </c>
+      <c r="AM3" s="0" t="str">
+        <v>Spanish II 1st</v>
+      </c>
+      <c r="AN3" s="0" t="str">
+        <v>Spanish II 4th</v>
+      </c>
+    </row>
+    <row r="4" spans="1:40" customFormat="false">
+      <c r="A4" s="0" t="str">
         <v>NOVICE ask/respond to  predictable, formulaic questions</v>
       </c>
+      <c r="B4" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="C4" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="D4" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="E4" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="F4" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="G4" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="H4" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="I4" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="J4" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="K4" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="L4" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="M4" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="N4" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="O4" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="P4" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="Q4" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="R4" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="S4" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="T4" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="U4" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="V4" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="W4" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="X4" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="Y4" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="Z4" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AA4" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AB4" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="AC4" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="AD4" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="AE4" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AF4" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AG4" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AH4" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AI4" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AJ4" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AK4" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="AL4" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AM4" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="AN4" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
     </row>
-    <row r="4" spans="1:1" customFormat="false">
-      <c r="A4" s="0" t="str">
+    <row r="5" spans="1:40" customFormat="false">
+      <c r="A5" s="0" t="str">
         <v>NOVICE list, name, identify</v>
       </c>
+      <c r="B5" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="C5" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="D5" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="E5" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="F5" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="G5" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="H5" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="I5" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="J5" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="K5" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="L5" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="M5" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="N5" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="O5" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="P5" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="Q5" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="R5" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="S5" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="T5" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="U5" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="V5" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="W5" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="X5" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="Y5" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="Z5" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AA5" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="AB5" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="AC5" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AD5" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AE5" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="AF5" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AG5" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AH5" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AI5" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="AJ5" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="AK5" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="AL5" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="AM5" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="AN5" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
     </row>
-    <row r="5" spans="1:1" customFormat="false">
-      <c r="A5" s="0" t="str">
+    <row r="6" spans="1:40" customFormat="false">
+      <c r="A6" s="0" t="str">
         <v>INTERMEDIATE ask, answer variety of questions</v>
       </c>
+      <c r="B6" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="C6" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="D6" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="E6" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="F6" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="G6" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="H6" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="I6" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="J6" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="K6" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="L6" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="M6" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="N6" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="O6" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="P6" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="Q6" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="R6" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="S6" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="T6" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="U6" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="V6" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="W6" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="X6" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="Y6" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="Z6" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="AA6" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AB6" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AC6" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AD6" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AE6" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AF6" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AG6" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="AH6" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AI6" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AJ6" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AK6" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="AL6" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AM6" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="AN6" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
     </row>
-    <row r="6" spans="1:1" customFormat="false">
-      <c r="A6" s="0" t="str">
+    <row r="7" spans="1:40" customFormat="false">
+      <c r="A7" s="0" t="str">
         <v>INTERMEDIATE initiate, maintain, end conversation for basic needs/transactions</v>
       </c>
+      <c r="B7" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="C7" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="D7" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="E7" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="F7" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="G7" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="H7" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="I7" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="J7" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="K7" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="L7" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="M7" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="N7" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="O7" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="P7" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="Q7" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="R7" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="S7" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="T7" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="U7" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="V7" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="W7" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="X7" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="Y7" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="Z7" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AA7" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AB7" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AC7" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AD7" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AE7" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AF7" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AG7" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="AH7" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AI7" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="AJ7" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AK7" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AL7" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="AM7" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AN7" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
     </row>
-    <row r="7" spans="1:1" customFormat="false">
-      <c r="A7" s="0" t="str">
+    <row r="8" spans="1:40" customFormat="false">
+      <c r="A8" s="0" t="str">
         <v>INTERMEDIATE communicate beyond "here &amp; now</v>
       </c>
+      <c r="B8" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="C8" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="D8" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="E8" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="F8" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="G8" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="H8" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="I8" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="J8" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="K8" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="L8" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="M8" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="N8" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="O8" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="P8" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="Q8" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="R8" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="S8" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="T8" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="U8" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="V8" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="W8" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="X8" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="Y8" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="Z8" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AA8" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AB8" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="AC8" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="AD8" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="AE8" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AF8" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AG8" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AH8" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AI8" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AJ8" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AK8" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="AL8" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AM8" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="AN8" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
     </row>
-    <row r="8" spans="1:1" customFormat="false">
-      <c r="A8" s="0" t="str">
+    <row r="9" spans="1:40" customFormat="false">
+      <c r="A9" s="0" t="str">
         <v>NOVICE practiced words, phrases, sentences</v>
       </c>
+      <c r="B9" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="C9" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="D9" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="E9" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="F9" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="G9" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="H9" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="I9" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="J9" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="K9" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="L9" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="M9" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="N9" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="O9" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="P9" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="Q9" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="R9" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="S9" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="T9" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="U9" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="V9" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="W9" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="X9" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="Y9" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="Z9" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AA9" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AB9" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AC9" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AD9" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="AE9" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="AF9" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AG9" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AH9" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AI9" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AJ9" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AK9" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="AL9" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AM9" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AN9" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
     </row>
-    <row r="9" spans="1:1" customFormat="false">
-      <c r="A9" s="0" t="str">
+    <row r="10" spans="1:40" customFormat="false">
+      <c r="A10" s="0" t="str">
         <v>NOVICE formulaic/memorized questions</v>
       </c>
+      <c r="B10" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="C10" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="D10" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="E10" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="F10" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="G10" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="H10" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="I10" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="J10" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="K10" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="L10" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="M10" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="N10" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="O10" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="P10" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="Q10" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="R10" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="S10" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="T10" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="U10" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="V10" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="W10" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="X10" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="Y10" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="Z10" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AA10" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AB10" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="AC10" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AD10" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="AE10" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="AF10" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AG10" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AH10" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="AI10" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AJ10" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AK10" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="AL10" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="AM10" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AN10" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
     </row>
-    <row r="10" spans="1:1" customFormat="false">
-      <c r="A10" s="0" t="str">
+    <row r="11" spans="1:40" customFormat="false">
+      <c r="A11" s="0" t="str">
         <v>INTERMEDIATE strings of sentences</v>
       </c>
+      <c r="B11" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="C11" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="D11" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="E11" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="F11" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="G11" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="H11" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="I11" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="J11" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="K11" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="L11" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="M11" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="N11" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="O11" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="P11" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="Q11" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="R11" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="S11" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="T11" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="U11" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="V11" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="W11" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="X11" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="Y11" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="Z11" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="AA11" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AB11" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AC11" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AD11" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AE11" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AF11" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="AG11" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AH11" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AI11" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AJ11" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AK11" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AL11" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AM11" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AN11" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
     </row>
-    <row r="11" spans="1:1" customFormat="false">
-      <c r="A11" s="0" t="str">
+    <row r="12" spans="1:40" customFormat="false">
+      <c r="A12" s="0" t="str">
         <v>INTERMEDIATE connected sentences</v>
       </c>
+      <c r="B12" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="C12" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="D12" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="E12" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="F12" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="G12" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="H12" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="I12" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="J12" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="K12" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="L12" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="M12" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="N12" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="O12" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="P12" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="Q12" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="R12" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="S12" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="T12" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="U12" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="V12" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="W12" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="X12" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="Y12" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="Z12" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AA12" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AB12" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AC12" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="AD12" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="AE12" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="AF12" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AG12" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="AH12" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AI12" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AJ12" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AK12" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AL12" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="AM12" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AN12" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
     </row>
-    <row r="12" spans="1:1" customFormat="false">
-      <c r="A12" s="0" t="str">
+    <row r="13" spans="1:40" customFormat="false">
+      <c r="A13" s="0" t="str">
         <v>INTERMEDIATE ask questions to initiate/ sustain conversation</v>
       </c>
+      <c r="B13" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="C13" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="D13" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="E13" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="F13" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="G13" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="H13" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="I13" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="J13" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="K13" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="L13" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="M13" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="N13" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="O13" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="P13" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="Q13" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="R13" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="S13" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="T13" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="U13" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="V13" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="W13" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="X13" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="Y13" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="Z13" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AA13" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AB13" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AC13" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AD13" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AE13" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="AF13" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="AG13" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="AH13" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AI13" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AJ13" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AK13" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AL13" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AM13" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="AN13" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
     </row>
-    <row r="13" spans="1:1" customFormat="false">
-      <c r="A13" s="0" t="str">
+    <row r="14" spans="1:40" customFormat="false">
+      <c r="A14" s="0" t="str">
         <v>NOVICE high-frequency</v>
       </c>
+      <c r="B14" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="C14" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="D14" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="E14" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="F14" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="G14" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="H14" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="I14" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="J14" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="K14" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="L14" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="M14" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="N14" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="O14" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="P14" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="Q14" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="R14" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="S14" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="T14" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="U14" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="V14" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="W14" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="X14" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="Y14" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="Z14" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AA14" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AB14" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="AC14" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AD14" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AE14" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AF14" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AG14" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AH14" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AI14" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AJ14" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="AK14" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AL14" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AM14" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AN14" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
     </row>
-    <row r="14" spans="1:1" customFormat="false">
-      <c r="A14" s="0" t="str">
+    <row r="15" spans="1:40" customFormat="false">
+      <c r="A15" s="0" t="str">
         <v>NOVICE formulaic</v>
       </c>
+      <c r="B15" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="C15" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="D15" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="E15" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="F15" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="G15" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="H15" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="I15" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="J15" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="K15" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="L15" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="M15" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="N15" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="O15" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="P15" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="Q15" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="R15" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="S15" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="T15" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="U15" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="V15" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="W15" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="X15" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="Y15" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="Z15" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AA15" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AB15" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="AC15" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AD15" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AE15" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="AF15" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AG15" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AH15" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="AI15" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="AJ15" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AK15" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AL15" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="AM15" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AN15" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
     </row>
-    <row r="15" spans="1:1" customFormat="false">
-      <c r="A15" s="0" t="str">
+    <row r="16" spans="1:40" customFormat="false">
+      <c r="A16" s="0" t="str">
         <v>NOVICE practiced</v>
       </c>
+      <c r="B16" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="C16" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="D16" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="E16" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="F16" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="G16" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="H16" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="I16" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="J16" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="K16" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="L16" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="M16" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="N16" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="O16" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="P16" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="Q16" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="R16" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="S16" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="T16" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="U16" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="V16" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="W16" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="X16" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="Y16" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="Z16" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AA16" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AB16" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AC16" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AD16" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="AE16" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AF16" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AG16" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AH16" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AI16" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AJ16" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AK16" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="AL16" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="AM16" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="AN16" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
     </row>
-    <row r="16" spans="1:1" customFormat="false">
-      <c r="A16" s="0" t="str">
+    <row r="17" spans="1:40" customFormat="false">
+      <c r="A17" s="0" t="str">
         <v>INTERMEDIATE familiar themes/topics</v>
       </c>
+      <c r="B17" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="C17" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="D17" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="E17" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="F17" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="G17" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="H17" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="I17" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="J17" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="K17" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="L17" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="M17" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="N17" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="O17" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="P17" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="Q17" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="R17" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="S17" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="T17" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="U17" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="V17" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="W17" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="X17" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="Y17" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="Z17" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AA17" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AB17" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AC17" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AD17" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="AE17" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AF17" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AG17" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AH17" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AI17" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AJ17" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="AK17" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="AL17" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="AM17" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AN17" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
     </row>
-    <row r="17" spans="1:1" customFormat="false">
-      <c r="A17" s="0" t="str">
+    <row r="18" spans="1:40" customFormat="false">
+      <c r="A18" s="0" t="str">
         <v>INTERMEDIATE personalized</v>
       </c>
+      <c r="B18" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="C18" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="D18" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="E18" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="F18" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="G18" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="H18" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="I18" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="J18" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="K18" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="L18" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="M18" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="N18" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="O18" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="P18" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="Q18" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="R18" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="S18" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="T18" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="U18" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="V18" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="W18" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="X18" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="Y18" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="Z18" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AA18" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AB18" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AC18" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AD18" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AE18" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AF18" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AG18" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AH18" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AI18" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="AJ18" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AK18" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AL18" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AM18" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AN18" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
     </row>
-    <row r="18" spans="1:1" customFormat="false">
-      <c r="A18" s="0" t="str">
+    <row r="19" spans="1:40" customFormat="false">
+      <c r="A19" s="0" t="str">
         <v>NOVICE imitate modeled words</v>
       </c>
+      <c r="B19" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="C19" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="D19" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="E19" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="F19" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="G19" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="H19" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="I19" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="J19" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="K19" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="L19" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="M19" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="N19" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="O19" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="P19" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="Q19" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="R19" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="S19" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="T19" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="U19" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="V19" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="W19" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="X19" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="Y19" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="Z19" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AA19" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AB19" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AC19" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AD19" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AE19" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AF19" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AG19" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AH19" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="AI19" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="AJ19" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AK19" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="AL19" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="AM19" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="AN19" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
     </row>
-    <row r="19" spans="1:1" customFormat="false">
-      <c r="A19" s="0" t="str">
+    <row r="20" spans="1:40" customFormat="false">
+      <c r="A20" s="0" t="str">
         <v>NOVICE use facial expressions, gestures</v>
       </c>
+      <c r="B20" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="C20" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="D20" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="E20" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="F20" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="G20" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="H20" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="I20" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="J20" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="K20" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="L20" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="M20" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="N20" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="O20" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="P20" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="Q20" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="R20" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="S20" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="T20" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="U20" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="V20" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="W20" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="X20" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="Y20" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="Z20" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AA20" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AB20" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AC20" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AD20" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AE20" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AF20" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="AG20" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="AH20" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AI20" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AJ20" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="AK20" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AL20" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="AM20" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AN20" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
     </row>
-    <row r="20" spans="1:1" customFormat="false">
-      <c r="A20" s="0" t="str">
+    <row r="21" spans="1:40" customFormat="false">
+      <c r="A21" s="0" t="str">
         <v>NOVICE resort to first language</v>
       </c>
+      <c r="B21" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="C21" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="D21" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="E21" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="F21" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="G21" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="H21" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="I21" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="J21" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="K21" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="L21" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="M21" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="N21" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="O21" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="P21" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="Q21" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="R21" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="S21" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="T21" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="U21" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="V21" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="W21" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="X21" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="Y21" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="Z21" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AA21" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AB21" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AC21" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AD21" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AE21" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AF21" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AG21" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AH21" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AI21" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AJ21" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AK21" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AL21" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AM21" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AN21" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
     </row>
-    <row r="21" spans="1:1" customFormat="false">
-      <c r="A21" s="0" t="str">
+    <row r="22" spans="1:40" customFormat="false">
+      <c r="A22" s="0" t="str">
         <v>NOVICE repeat/request repetition</v>
       </c>
+      <c r="B22" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="C22" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="D22" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="E22" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="F22" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="G22" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="H22" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="I22" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="J22" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="K22" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="L22" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="M22" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="N22" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="O22" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="P22" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="Q22" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="R22" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="S22" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="T22" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="U22" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="V22" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="W22" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="X22" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="Y22" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="Z22" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AA22" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AB22" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AC22" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="AD22" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AE22" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AF22" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AG22" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AH22" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="AI22" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AJ22" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AK22" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AL22" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AM22" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AN22" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
     </row>
-    <row r="22" spans="1:1" customFormat="false">
-      <c r="A22" s="0" t="str">
+    <row r="23" spans="1:40" customFormat="false">
+      <c r="A23" s="0" t="str">
         <v>NOVICE indicate lack of understanding</v>
       </c>
+      <c r="B23" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="C23" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="D23" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="E23" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="F23" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="G23" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="H23" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="I23" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="J23" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="K23" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="L23" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="M23" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="N23" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="O23" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="P23" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="Q23" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="R23" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="S23" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="T23" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="U23" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="V23" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="W23" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="X23" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="Y23" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="Z23" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AA23" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AB23" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AC23" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AD23" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AE23" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AF23" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="AG23" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="AH23" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AI23" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AJ23" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AK23" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AL23" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AM23" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AN23" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
     </row>
-    <row r="23" spans="1:1" customFormat="false">
-      <c r="A23" s="0" t="str">
+    <row r="24" spans="1:40" customFormat="false">
+      <c r="A24" s="0" t="str">
         <v>INTERMEDIATE ask questions, request clarification</v>
       </c>
+      <c r="B24" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="C24" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="D24" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="E24" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="F24" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="G24" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="H24" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="I24" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="J24" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="K24" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="L24" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="M24" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="N24" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="O24" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="P24" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="Q24" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="R24" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="S24" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="T24" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="U24" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="V24" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="W24" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="X24" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="Y24" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="Z24" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AA24" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AB24" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AC24" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AD24" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="AE24" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AF24" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AG24" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="AH24" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AI24" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AJ24" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AK24" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AL24" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AM24" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AN24" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
     </row>
-    <row r="24" spans="1:1" customFormat="false">
-      <c r="A24" s="0" t="str">
+    <row r="25" spans="1:40" customFormat="false">
+      <c r="A25" s="0" t="str">
         <v>INTERMEDIATE self-correct or restate when not understood</v>
       </c>
+      <c r="B25" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="C25" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="D25" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="E25" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="F25" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="G25" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="H25" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="I25" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="J25" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="K25" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="L25" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="M25" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="N25" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="O25" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="P25" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="Q25" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="R25" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="S25" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="T25" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="U25" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="V25" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="W25" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="X25" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="Y25" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="Z25" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AA25" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AB25" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="AC25" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AD25" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="AE25" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AF25" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AG25" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AH25" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AI25" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AJ25" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AK25" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="AL25" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="AM25" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AN25" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
     </row>
-    <row r="25" spans="1:1" customFormat="false">
-      <c r="A25" s="0" t="str">
+    <row r="26" spans="1:40" customFormat="false">
+      <c r="A26" s="0" t="str">
         <v>INTERMEDIATE circumlocute</v>
+      </c>
+      <c r="B26" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="C26" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="D26" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="E26" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="F26" s="0" t="str">
+        <v xml:space="preserve"> A-C</v>
+      </c>
+      <c r="G26" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="H26" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="I26" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="J26" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="K26" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="L26" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="M26" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="N26" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="O26" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="P26" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="Q26" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="R26" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="S26" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="T26" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="U26" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="V26" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="W26" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="X26" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="Y26" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="Z26" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AA26" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AB26" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AC26" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AD26" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AE26" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AF26" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="AG26" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AH26" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AI26" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
+      </c>
+      <c r="AJ26" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AK26" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AL26" s="0" t="str">
+        <v xml:space="preserve"> -B-</v>
+      </c>
+      <c r="AM26" s="0" t="str">
+        <v xml:space="preserve"> ABC</v>
+      </c>
+      <c r="AN26" s="0" t="str">
+        <v xml:space="preserve"> ---</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final, unless she needs something else
</commit_message>
<xml_diff>
--- a/speaking.xlsx
+++ b/speaking.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="302" count="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="306" count="306">
   <si>
     <t>Timestamp</t>
   </si>
@@ -929,6 +929,18 @@
   </si>
   <si>
     <t>Be able to have the courage to speak.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A-C</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ABC</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ---</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -B-</t>
   </si>
 </sst>
 </file>
@@ -938,7 +950,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <name val="Arial"/>
       <color rgb="FF000000"/>
@@ -951,6 +963,12 @@
     <font>
       <name val="Arial"/>
       <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <u val="1"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <color theme="10"/>
       <sz val="10"/>
       <u val="1"/>
     </font>
@@ -972,16 +990,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -11998,13 +12019,13 @@
   <dimension ref="B1:AN26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="A1:AN27"/>
+      <selection activeCell="AN3" sqref="AN3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" customWidth="1"/>
+    <col min="1" max="1" width="69.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:40" customFormat="false">
@@ -12369,7 +12390,7 @@
         <v>NOVICE ask/respond to  predictable, formulaic questions</v>
       </c>
       <c r="B4" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="C4" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -12378,28 +12399,28 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="E4" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="F4" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="G4" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="H4" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="I4" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="J4" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="K4" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="L4" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="M4" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -12411,13 +12432,13 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="P4" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="Q4" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="R4" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="S4" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -12435,7 +12456,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="X4" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="Y4" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -12444,16 +12465,16 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AA4" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AB4" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="AC4" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="AD4" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="AE4" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -12462,7 +12483,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AG4" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AH4" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -12471,19 +12492,19 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AJ4" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AK4" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="AL4" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AM4" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="AN4" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
     </row>
     <row r="5" spans="1:40" customFormat="false">
@@ -12491,7 +12512,7 @@
         <v>NOVICE list, name, identify</v>
       </c>
       <c r="B5" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="C5" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -12500,55 +12521,55 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="E5" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="F5" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="G5" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="H5" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="I5" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="J5" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="K5" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="L5" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="M5" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="N5" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="O5" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="P5" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="Q5" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="R5" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="S5" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="T5" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="U5" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="V5" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -12557,31 +12578,31 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="X5" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="Y5" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="Z5" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AA5" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="AB5" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="AC5" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AD5" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AE5" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="AF5" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AG5" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -12590,22 +12611,22 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AI5" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="AJ5" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="AK5" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="AL5" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="AM5" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="AN5" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
     </row>
     <row r="6" spans="1:40" customFormat="false">
@@ -12616,7 +12637,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="C6" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="D6" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -12625,7 +12646,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="F6" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="G6" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -12637,7 +12658,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="J6" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="K6" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -12646,7 +12667,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="M6" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="N6" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -12655,7 +12676,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="P6" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="Q6" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -12667,13 +12688,13 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="T6" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="U6" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="V6" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="W6" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -12685,7 +12706,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="Z6" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="AA6" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -12700,13 +12721,13 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AE6" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AF6" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AG6" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="AH6" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -12718,13 +12739,13 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AK6" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="AL6" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AM6" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="AN6" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -12744,19 +12765,19 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="E7" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="F7" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="G7" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="H7" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="I7" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="J7" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -12765,19 +12786,19 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="L7" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="M7" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="N7" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="O7" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="P7" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="Q7" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -12786,16 +12807,16 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="S7" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="T7" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="U7" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="V7" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="W7" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -12828,13 +12849,13 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AG7" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="AH7" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AI7" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="AJ7" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -12843,13 +12864,13 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AL7" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="AM7" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AN7" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
     </row>
     <row r="8" spans="1:40" customFormat="false">
@@ -12857,121 +12878,121 @@
         <v>INTERMEDIATE communicate beyond "here &amp; now</v>
       </c>
       <c r="B8" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="C8" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="D8" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="E8" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="F8" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="G8" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="H8" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="I8" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="J8" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="K8" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="L8" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="M8" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="N8" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="O8" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="P8" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="Q8" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="R8" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="S8" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="T8" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="U8" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="V8" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="W8" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="X8" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="Y8" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="Z8" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AA8" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AB8" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="AC8" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="AD8" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="AE8" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AF8" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AG8" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AH8" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AI8" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AJ8" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AK8" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="AL8" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AM8" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="AN8" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
     </row>
     <row r="9" spans="1:40" customFormat="false">
@@ -12988,13 +13009,13 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="E9" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="F9" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="G9" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="H9" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13006,10 +13027,10 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="K9" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="L9" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="M9" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13021,19 +13042,19 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="P9" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="Q9" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="R9" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="S9" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="T9" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="U9" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13045,7 +13066,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="X9" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="Y9" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13054,7 +13075,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AA9" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AB9" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13063,10 +13084,10 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AD9" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="AE9" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="AF9" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13081,10 +13102,10 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AJ9" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AK9" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="AL9" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13101,7 +13122,7 @@
         <v>NOVICE formulaic/memorized questions</v>
       </c>
       <c r="B10" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="C10" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13110,10 +13131,10 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="E10" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="F10" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="G10" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13125,37 +13146,37 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="J10" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="K10" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="L10" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="M10" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="N10" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="O10" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="P10" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="Q10" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="R10" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="S10" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="T10" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="U10" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13167,28 +13188,28 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="X10" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="Y10" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="Z10" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AA10" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AB10" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="AC10" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AD10" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="AE10" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="AF10" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13197,25 +13218,25 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AH10" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="AI10" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AJ10" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AK10" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="AL10" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="AM10" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AN10" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
     </row>
     <row r="11" spans="1:40" customFormat="false">
@@ -13226,7 +13247,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="C11" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="D11" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13235,13 +13256,13 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="F11" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="G11" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="H11" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="I11" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13253,40 +13274,40 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="L11" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="M11" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="N11" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="O11" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="P11" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="Q11" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="R11" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="S11" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="T11" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="U11" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="V11" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="W11" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="X11" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13295,7 +13316,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="Z11" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="AA11" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13313,7 +13334,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AF11" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="AG11" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13325,19 +13346,19 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AJ11" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AK11" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AL11" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AM11" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AN11" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
     </row>
     <row r="12" spans="1:40" customFormat="false">
@@ -13345,10 +13366,10 @@
         <v>INTERMEDIATE connected sentences</v>
       </c>
       <c r="B12" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="C12" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="D12" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13357,37 +13378,37 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="F12" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="G12" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="H12" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="I12" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="J12" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="K12" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="L12" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="M12" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="N12" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="O12" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="P12" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="Q12" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13396,16 +13417,16 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="S12" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="T12" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="U12" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="V12" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="W12" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13417,7 +13438,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="Z12" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AA12" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13426,40 +13447,40 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AC12" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="AD12" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="AE12" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="AF12" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AG12" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="AH12" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AI12" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AJ12" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AK12" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AL12" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="AM12" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AN12" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
     </row>
     <row r="13" spans="1:40" customFormat="false">
@@ -13470,34 +13491,34 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="C13" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="D13" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="E13" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="F13" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="G13" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="H13" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="I13" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="J13" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="K13" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="L13" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="M13" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13509,7 +13530,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="P13" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="Q13" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13536,7 +13557,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="Y13" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="Z13" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13554,16 +13575,16 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AE13" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="AF13" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="AG13" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="AH13" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AI13" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13578,10 +13599,10 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AM13" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="AN13" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
     </row>
     <row r="14" spans="1:40" customFormat="false">
@@ -13589,61 +13610,61 @@
         <v>NOVICE high-frequency</v>
       </c>
       <c r="B14" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="C14" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="D14" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="E14" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="F14" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="G14" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="H14" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="I14" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="J14" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="K14" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="L14" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="M14" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="N14" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="O14" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="P14" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="Q14" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="R14" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="S14" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="T14" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="U14" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13652,58 +13673,58 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="W14" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="X14" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="Y14" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="Z14" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AA14" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AB14" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="AC14" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AD14" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AE14" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AF14" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AG14" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AH14" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AI14" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AJ14" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="AK14" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AL14" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AM14" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AN14" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
     </row>
     <row r="15" spans="1:40" customFormat="false">
@@ -13711,7 +13732,7 @@
         <v>NOVICE formulaic</v>
       </c>
       <c r="B15" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="C15" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13720,16 +13741,16 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="E15" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="F15" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="G15" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="H15" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="I15" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13738,34 +13759,34 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="K15" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="L15" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="M15" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="N15" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="O15" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="P15" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="Q15" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="R15" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="S15" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="T15" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="U15" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13777,55 +13798,55 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="X15" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="Y15" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="Z15" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AA15" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AB15" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="AC15" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AD15" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AE15" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="AF15" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AG15" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AH15" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="AI15" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="AJ15" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AK15" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AL15" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="AM15" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AN15" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
     </row>
     <row r="16" spans="1:40" customFormat="false">
@@ -13836,16 +13857,16 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="C16" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="D16" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="E16" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="F16" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="G16" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13854,16 +13875,16 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="I16" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="J16" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="K16" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="L16" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="M16" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13887,7 +13908,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="T16" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="U16" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13899,13 +13920,13 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="X16" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="Y16" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="Z16" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AA16" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13917,7 +13938,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AD16" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="AE16" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13929,22 +13950,22 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AH16" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AI16" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AJ16" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AK16" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="AL16" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="AM16" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="AN16" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13967,7 +13988,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="F17" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="G17" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13985,7 +14006,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="L17" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="M17" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13997,7 +14018,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="P17" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="Q17" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -14009,13 +14030,13 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="T17" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="U17" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="V17" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="W17" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -14024,7 +14045,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="Y17" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="Z17" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -14039,7 +14060,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AD17" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="AE17" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -14057,13 +14078,13 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AJ17" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="AK17" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="AL17" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="AM17" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -14080,16 +14101,16 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="C18" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="D18" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="E18" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="F18" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="G18" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -14098,10 +14119,10 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="I18" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="J18" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="K18" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -14116,28 +14137,28 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="O18" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="P18" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="Q18" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="R18" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="S18" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="T18" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="U18" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="V18" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="W18" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -14146,7 +14167,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="Y18" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="Z18" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -14167,16 +14188,16 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AF18" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AG18" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AH18" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AI18" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="AJ18" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -14191,7 +14212,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AN18" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
     </row>
     <row r="19" spans="1:40" customFormat="false">
@@ -14202,40 +14223,40 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="C19" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="D19" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="E19" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="F19" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="G19" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="H19" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="I19" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="J19" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="K19" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="L19" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="M19" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="N19" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="O19" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -14244,7 +14265,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="Q19" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="R19" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -14262,13 +14283,13 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="W19" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="X19" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="Y19" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="Z19" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -14277,43 +14298,43 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AB19" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AC19" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AD19" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AE19" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AF19" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AG19" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AH19" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="AI19" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="AJ19" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AK19" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="AL19" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="AM19" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="AN19" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
     </row>
     <row r="20" spans="1:40" customFormat="false">
@@ -14321,121 +14342,121 @@
         <v>NOVICE use facial expressions, gestures</v>
       </c>
       <c r="B20" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="C20" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="D20" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="E20" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="F20" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="G20" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="H20" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="I20" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="J20" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="K20" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="L20" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="M20" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="N20" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="O20" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="P20" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="Q20" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="R20" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="S20" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="T20" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="U20" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="V20" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="W20" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="X20" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="Y20" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="Z20" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AA20" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AB20" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AC20" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AD20" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AE20" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AF20" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="AG20" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="AH20" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AI20" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AJ20" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="AK20" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AL20" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="AM20" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AN20" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
     </row>
     <row r="21" spans="1:40" customFormat="false">
@@ -14443,118 +14464,118 @@
         <v>NOVICE resort to first language</v>
       </c>
       <c r="B21" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="C21" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="D21" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="E21" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="F21" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="G21" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="H21" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="I21" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="J21" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="K21" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="L21" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="M21" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="N21" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="O21" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="P21" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="Q21" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="R21" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="S21" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="T21" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="U21" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="V21" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="W21" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="X21" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="Y21" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="Z21" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AA21" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AB21" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AC21" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AD21" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AE21" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AF21" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AG21" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AH21" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AI21" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AJ21" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AK21" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AL21" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AM21" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AN21" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -14565,121 +14586,121 @@
         <v>NOVICE repeat/request repetition</v>
       </c>
       <c r="B22" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="C22" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="D22" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="E22" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="F22" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="G22" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="H22" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="I22" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="J22" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="K22" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="L22" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="M22" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="N22" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="O22" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="P22" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="Q22" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="R22" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="S22" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="T22" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="U22" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="V22" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="W22" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="X22" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="Y22" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="Z22" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AA22" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AB22" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AC22" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="AD22" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AE22" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AF22" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AG22" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AH22" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="AI22" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AJ22" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AK22" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AL22" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AM22" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AN22" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
     </row>
     <row r="23" spans="1:40" customFormat="false">
@@ -14687,121 +14708,121 @@
         <v>NOVICE indicate lack of understanding</v>
       </c>
       <c r="B23" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="C23" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="D23" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="E23" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="F23" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="G23" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="H23" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="I23" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="J23" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="K23" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="L23" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="M23" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="N23" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="O23" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="P23" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="Q23" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="R23" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="S23" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="T23" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="U23" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="V23" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="W23" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="X23" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="Y23" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="Z23" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AA23" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AB23" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AC23" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AD23" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AE23" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AF23" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="AG23" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="AH23" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AI23" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AJ23" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AK23" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AL23" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AM23" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AN23" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
     </row>
     <row r="24" spans="1:40" customFormat="false">
@@ -14812,19 +14833,19 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="C24" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="D24" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="E24" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="F24" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="G24" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="H24" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -14833,52 +14854,52 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="J24" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="K24" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="L24" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="M24" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="N24" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="O24" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="P24" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="Q24" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="R24" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="S24" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="T24" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="U24" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="V24" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="W24" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="X24" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="Y24" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="Z24" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -14893,37 +14914,37 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AD24" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="AE24" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AF24" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AG24" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="AH24" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AI24" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AJ24" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AK24" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AL24" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AM24" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AN24" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
     </row>
     <row r="25" spans="1:40" customFormat="false">
@@ -14931,22 +14952,22 @@
         <v>INTERMEDIATE self-correct or restate when not understood</v>
       </c>
       <c r="B25" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="C25" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="D25" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="E25" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="F25" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="G25" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="H25" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -14961,19 +14982,19 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="L25" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="M25" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="N25" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="O25" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="P25" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="Q25" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -14982,46 +15003,46 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="S25" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="T25" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="U25" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="V25" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="W25" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="X25" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="Y25" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="Z25" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AA25" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AB25" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="AC25" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AD25" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="AE25" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AF25" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AG25" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -15030,22 +15051,22 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AI25" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AJ25" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AK25" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="AL25" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="AM25" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AN25" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
     </row>
     <row r="26" spans="1:40" customFormat="false">
@@ -15053,10 +15074,10 @@
         <v>INTERMEDIATE circumlocute</v>
       </c>
       <c r="B26" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="C26" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="D26" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -15065,16 +15086,16 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="F26" s="0" t="str">
-        <v xml:space="preserve"> A-C</v>
+        <v xml:space="preserve"> A C</v>
       </c>
       <c r="G26" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="H26" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="I26" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="J26" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -15083,10 +15104,10 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="L26" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="M26" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="N26" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -15095,37 +15116,37 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="P26" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="Q26" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="R26" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="S26" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="T26" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="U26" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="V26" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="W26" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="X26" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="Y26" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="Z26" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AA26" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -15143,16 +15164,16 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AF26" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="AG26" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AH26" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AI26" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
       <c r="AJ26" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -15161,16 +15182,54 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AL26" s="0" t="str">
-        <v xml:space="preserve"> -B-</v>
+        <v xml:space="preserve">  B </v>
       </c>
       <c r="AM26" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AN26" s="0" t="str">
-        <v xml:space="preserve"> ---</v>
+        <v xml:space="preserve">    </v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId2"/>
+    <hyperlink ref="D2" r:id="rId3"/>
+    <hyperlink ref="E2" r:id="rId4"/>
+    <hyperlink ref="F2" r:id="rId5"/>
+    <hyperlink ref="G2" r:id="rId6"/>
+    <hyperlink ref="H2" r:id="rId7"/>
+    <hyperlink ref="I2" r:id="rId8"/>
+    <hyperlink ref="J2" r:id="rId9"/>
+    <hyperlink ref="K2" r:id="rId10"/>
+    <hyperlink ref="L2" r:id="rId11"/>
+    <hyperlink ref="M2" r:id="rId12"/>
+    <hyperlink ref="N2" r:id="rId13"/>
+    <hyperlink ref="O2" r:id="rId14"/>
+    <hyperlink ref="Q2" r:id="rId15"/>
+    <hyperlink ref="R2" r:id="rId16"/>
+    <hyperlink ref="S2" r:id="rId17"/>
+    <hyperlink ref="U2" r:id="rId18"/>
+    <hyperlink ref="V2" r:id="rId19"/>
+    <hyperlink ref="W2" r:id="rId20"/>
+    <hyperlink ref="X2" r:id="rId21"/>
+    <hyperlink ref="Y2" r:id="rId22"/>
+    <hyperlink ref="Z2" r:id="rId23"/>
+    <hyperlink ref="AB2" r:id="rId24"/>
+    <hyperlink ref="AC2" r:id="rId25"/>
+    <hyperlink ref="AD2" r:id="rId26"/>
+    <hyperlink ref="AE2" r:id="rId27"/>
+    <hyperlink ref="AF2" r:id="rId28"/>
+    <hyperlink ref="AG2" r:id="rId29"/>
+    <hyperlink ref="AH2" r:id="rId30"/>
+    <hyperlink ref="AI2" r:id="rId31"/>
+    <hyperlink ref="AJ2" r:id="rId32"/>
+    <hyperlink ref="AK2" r:id="rId33"/>
+    <hyperlink ref="AL2" r:id="rId34"/>
+    <hyperlink ref="AM2" r:id="rId35"/>
+    <hyperlink ref="AN2" r:id="rId36"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Bug Fixes, Time Inclusion
</commit_message>
<xml_diff>
--- a/speaking.xlsx
+++ b/speaking.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="306" count="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="302" count="302">
   <si>
     <t>Timestamp</t>
   </si>
@@ -929,18 +929,6 @@
   </si>
   <si>
     <t>Be able to have the courage to speak.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> A-C</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ABC</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ---</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> -B-</t>
   </si>
 </sst>
 </file>
@@ -950,7 +938,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <name val="Arial"/>
       <color rgb="FF000000"/>
@@ -963,12 +951,6 @@
     <font>
       <name val="Arial"/>
       <color rgb="FF0000FF"/>
-      <sz val="10"/>
-      <u val="1"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <color theme="10"/>
       <sz val="10"/>
       <u val="1"/>
     </font>
@@ -990,19 +972,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1321,13 +1300,15 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" customWidth="1"/>
-    <col min="2" max="88" width="21.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="21.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
+    <col min="7" max="88" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:88" customFormat="false" ht="15.75" customHeight="1">
@@ -12019,7 +12000,7 @@
   <dimension ref="B1:AN26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AN3" sqref="AN3"/>
+      <selection activeCell="A26" sqref="A1:AO26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.7109375" defaultRowHeight="12.75"/>
@@ -12266,7 +12247,10 @@
         <v>http://gecwestonpespanol.blogspot.com/p/speaking.html</v>
       </c>
     </row>
-    <row r="3" spans="2:40" customFormat="false">
+    <row r="3" spans="1:40" customFormat="false">
+      <c r="A3" s="0" t="str">
+        <v>NOVICE ask/respond to  predictable, formulaic questions</v>
+      </c>
       <c r="B3" s="0" t="str">
         <v>Spanish II 1st</v>
       </c>
@@ -12396,7 +12380,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="D4" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="E4" s="0" t="str">
         <v xml:space="preserve">    </v>
@@ -12408,25 +12392,25 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="H4" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="I4" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="J4" s="0" t="str">
         <v xml:space="preserve"> A C</v>
       </c>
       <c r="K4" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="L4" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="M4" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="N4" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="O4" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -12435,10 +12419,10 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="Q4" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="R4" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="S4" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -12447,7 +12431,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="U4" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="V4" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -12462,7 +12446,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="Z4" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="AA4" s="0" t="str">
         <v xml:space="preserve">    </v>
@@ -12495,16 +12479,16 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="AK4" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="AL4" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AM4" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="AN4" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
     </row>
     <row r="5" spans="1:40" customFormat="false">
@@ -12524,16 +12508,16 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="F5" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="G5" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="H5" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="I5" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="J5" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -12542,7 +12526,7 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="L5" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="M5" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -12557,13 +12541,13 @@
         <v xml:space="preserve">  B </v>
       </c>
       <c r="Q5" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="R5" s="0" t="str">
         <v xml:space="preserve">  B </v>
       </c>
       <c r="S5" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="T5" s="0" t="str">
         <v xml:space="preserve">    </v>
@@ -12578,13 +12562,13 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="X5" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="Y5" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="Z5" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="AA5" s="0" t="str">
         <v xml:space="preserve"> A C</v>
@@ -12608,22 +12592,22 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AH5" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="AI5" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="AJ5" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="AK5" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="AL5" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="AM5" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="AN5" s="0" t="str">
         <v xml:space="preserve">    </v>
@@ -12634,13 +12618,13 @@
         <v>INTERMEDIATE ask, answer variety of questions</v>
       </c>
       <c r="B6" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="C6" s="0" t="str">
         <v xml:space="preserve"> A C</v>
       </c>
       <c r="D6" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="E6" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -12655,7 +12639,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="I6" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="J6" s="0" t="str">
         <v xml:space="preserve"> A C</v>
@@ -12667,7 +12651,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="M6" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="N6" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -12682,31 +12666,31 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="R6" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="S6" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="T6" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="U6" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="V6" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="W6" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="X6" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="Y6" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="Z6" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="AA6" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -12721,13 +12705,13 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AE6" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="AF6" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AG6" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="AH6" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -12739,7 +12723,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AK6" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="AL6" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -12748,7 +12732,7 @@
         <v xml:space="preserve"> A C</v>
       </c>
       <c r="AN6" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
     </row>
     <row r="7" spans="1:40" customFormat="false">
@@ -12765,13 +12749,13 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="E7" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="F7" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="G7" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="H7" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -12789,7 +12773,7 @@
         <v xml:space="preserve">  B </v>
       </c>
       <c r="M7" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="N7" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -12804,10 +12788,10 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="R7" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="S7" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="T7" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -12816,19 +12800,19 @@
         <v xml:space="preserve"> A C</v>
       </c>
       <c r="V7" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="W7" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="X7" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="Y7" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="Z7" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="AA7" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -12852,7 +12836,7 @@
         <v xml:space="preserve"> A C</v>
       </c>
       <c r="AH7" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="AI7" s="0" t="str">
         <v xml:space="preserve"> A C</v>
@@ -12864,7 +12848,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AL7" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="AM7" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -12884,16 +12868,16 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="D8" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="E8" s="0" t="str">
         <v xml:space="preserve">    </v>
       </c>
       <c r="F8" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="G8" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="H8" s="0" t="str">
         <v xml:space="preserve"> A C</v>
@@ -12902,7 +12886,7 @@
         <v xml:space="preserve">  B </v>
       </c>
       <c r="J8" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="K8" s="0" t="str">
         <v xml:space="preserve">    </v>
@@ -12926,10 +12910,10 @@
         <v xml:space="preserve">  B </v>
       </c>
       <c r="R8" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="S8" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="T8" s="0" t="str">
         <v xml:space="preserve"> A C</v>
@@ -12944,7 +12928,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="X8" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="Y8" s="0" t="str">
         <v xml:space="preserve"> A C</v>
@@ -12956,7 +12940,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AB8" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="AC8" s="0" t="str">
         <v xml:space="preserve">  B </v>
@@ -12974,7 +12958,7 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="AH8" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="AI8" s="0" t="str">
         <v xml:space="preserve">    </v>
@@ -12986,10 +12970,10 @@
         <v xml:space="preserve">  B </v>
       </c>
       <c r="AL8" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="AM8" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="AN8" s="0" t="str">
         <v xml:space="preserve">    </v>
@@ -13000,7 +12984,7 @@
         <v>NOVICE practiced words, phrases, sentences</v>
       </c>
       <c r="B9" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="C9" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13036,7 +13020,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="N9" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="O9" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13045,16 +13029,16 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="Q9" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="R9" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="S9" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="T9" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="U9" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13069,7 +13053,7 @@
         <v xml:space="preserve"> A C</v>
       </c>
       <c r="Y9" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="Z9" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13084,7 +13068,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AD9" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="AE9" s="0" t="str">
         <v xml:space="preserve">  B </v>
@@ -13105,16 +13089,16 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="AK9" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="AL9" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AM9" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="AN9" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
     </row>
     <row r="10" spans="1:40" customFormat="false">
@@ -13122,28 +13106,28 @@
         <v>NOVICE formulaic/memorized questions</v>
       </c>
       <c r="B10" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="C10" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="D10" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="E10" s="0" t="str">
         <v xml:space="preserve">    </v>
       </c>
       <c r="F10" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="G10" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="H10" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="I10" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="J10" s="0" t="str">
         <v xml:space="preserve"> A C</v>
@@ -13152,22 +13136,22 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="L10" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="M10" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="N10" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="O10" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="P10" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="Q10" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="R10" s="0" t="str">
         <v xml:space="preserve">  B </v>
@@ -13197,10 +13181,10 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="AA10" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="AB10" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="AC10" s="0" t="str">
         <v xml:space="preserve">    </v>
@@ -13209,7 +13193,7 @@
         <v xml:space="preserve">  B </v>
       </c>
       <c r="AE10" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="AF10" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13218,7 +13202,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AH10" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="AI10" s="0" t="str">
         <v xml:space="preserve">    </v>
@@ -13227,13 +13211,13 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="AK10" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="AL10" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="AM10" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="AN10" s="0" t="str">
         <v xml:space="preserve">    </v>
@@ -13244,7 +13228,7 @@
         <v>INTERMEDIATE strings of sentences</v>
       </c>
       <c r="B11" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="C11" s="0" t="str">
         <v xml:space="preserve">    </v>
@@ -13268,13 +13252,13 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="J11" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="K11" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="L11" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="M11" s="0" t="str">
         <v xml:space="preserve"> A C</v>
@@ -13292,7 +13276,7 @@
         <v xml:space="preserve">  B </v>
       </c>
       <c r="R11" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="S11" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13301,10 +13285,10 @@
         <v xml:space="preserve"> A C</v>
       </c>
       <c r="U11" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="V11" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="W11" s="0" t="str">
         <v xml:space="preserve">  B </v>
@@ -13349,10 +13333,10 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="AK11" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="AL11" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="AM11" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13366,16 +13350,16 @@
         <v>INTERMEDIATE connected sentences</v>
       </c>
       <c r="B12" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="C12" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="D12" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="E12" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="F12" s="0" t="str">
         <v xml:space="preserve"> A C</v>
@@ -13390,13 +13374,13 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="J12" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="K12" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="L12" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="M12" s="0" t="str">
         <v xml:space="preserve"> A C</v>
@@ -13408,7 +13392,7 @@
         <v xml:space="preserve"> A C</v>
       </c>
       <c r="P12" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="Q12" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13438,7 +13422,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="Z12" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="AA12" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13447,7 +13431,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AC12" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="AD12" s="0" t="str">
         <v xml:space="preserve">  B </v>
@@ -13459,7 +13443,7 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="AG12" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="AH12" s="0" t="str">
         <v xml:space="preserve">    </v>
@@ -13471,10 +13455,10 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AK12" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="AL12" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="AM12" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13494,16 +13478,16 @@
         <v xml:space="preserve"> A C</v>
       </c>
       <c r="D13" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="E13" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="F13" s="0" t="str">
         <v xml:space="preserve"> A C</v>
       </c>
       <c r="G13" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="H13" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13518,13 +13502,13 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="L13" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="M13" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="N13" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="O13" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13536,7 +13520,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="R13" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="S13" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13554,13 +13538,13 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="X13" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="Y13" s="0" t="str">
         <v xml:space="preserve"> A C</v>
       </c>
       <c r="Z13" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="AA13" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13578,10 +13562,10 @@
         <v xml:space="preserve"> A C</v>
       </c>
       <c r="AF13" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="AG13" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="AH13" s="0" t="str">
         <v xml:space="preserve">    </v>
@@ -13602,7 +13586,7 @@
         <v xml:space="preserve"> A C</v>
       </c>
       <c r="AN13" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
     </row>
     <row r="14" spans="1:40" customFormat="false">
@@ -13622,7 +13606,7 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="F14" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="G14" s="0" t="str">
         <v xml:space="preserve">    </v>
@@ -13643,7 +13627,7 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="M14" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="N14" s="0" t="str">
         <v xml:space="preserve">    </v>
@@ -13658,13 +13642,13 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="R14" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="S14" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="T14" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="U14" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13673,7 +13657,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="W14" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="X14" s="0" t="str">
         <v xml:space="preserve">    </v>
@@ -13688,7 +13672,7 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="AB14" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="AC14" s="0" t="str">
         <v xml:space="preserve">    </v>
@@ -13712,16 +13696,16 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="AJ14" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="AK14" s="0" t="str">
         <v xml:space="preserve">    </v>
       </c>
       <c r="AL14" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="AM14" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="AN14" s="0" t="str">
         <v xml:space="preserve">    </v>
@@ -13732,7 +13716,7 @@
         <v>NOVICE formulaic</v>
       </c>
       <c r="B15" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="C15" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13750,7 +13734,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="H15" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="I15" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13789,13 +13773,13 @@
         <v xml:space="preserve">  B </v>
       </c>
       <c r="U15" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="V15" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="W15" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="X15" s="0" t="str">
         <v xml:space="preserve">    </v>
@@ -13804,7 +13788,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="Z15" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="AA15" s="0" t="str">
         <v xml:space="preserve">    </v>
@@ -13819,7 +13803,7 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="AE15" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="AF15" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13828,10 +13812,10 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="AH15" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="AI15" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="AJ15" s="0" t="str">
         <v xml:space="preserve">    </v>
@@ -13840,7 +13824,7 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="AL15" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="AM15" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13863,22 +13847,22 @@
         <v xml:space="preserve"> A C</v>
       </c>
       <c r="E16" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="F16" s="0" t="str">
         <v xml:space="preserve"> A C</v>
       </c>
       <c r="G16" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="H16" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="I16" s="0" t="str">
         <v xml:space="preserve"> A C</v>
       </c>
       <c r="J16" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="K16" s="0" t="str">
         <v xml:space="preserve">    </v>
@@ -13899,7 +13883,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="Q16" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="R16" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13911,19 +13895,19 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="U16" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="V16" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="W16" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="X16" s="0" t="str">
         <v xml:space="preserve"> A C</v>
       </c>
       <c r="Y16" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="Z16" s="0" t="str">
         <v xml:space="preserve">    </v>
@@ -13938,7 +13922,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AD16" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="AE16" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -13953,22 +13937,22 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="AI16" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="AJ16" s="0" t="str">
         <v xml:space="preserve">    </v>
       </c>
       <c r="AK16" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="AL16" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="AM16" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="AN16" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
     </row>
     <row r="17" spans="1:40" customFormat="false">
@@ -14036,7 +14020,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="V17" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="W17" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -14078,10 +14062,10 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AJ17" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="AK17" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="AL17" s="0" t="str">
         <v xml:space="preserve"> A C</v>
@@ -14090,7 +14074,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AN17" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
     </row>
     <row r="18" spans="1:40" customFormat="false">
@@ -14101,7 +14085,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="C18" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="D18" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -14119,10 +14103,10 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="I18" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="J18" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="K18" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -14131,13 +14115,13 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="M18" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="N18" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="O18" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="P18" s="0" t="str">
         <v xml:space="preserve">    </v>
@@ -14149,28 +14133,28 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="S18" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="T18" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="U18" s="0" t="str">
         <v xml:space="preserve">    </v>
       </c>
       <c r="V18" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="W18" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="X18" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="Y18" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="Z18" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="AA18" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -14191,13 +14175,13 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="AG18" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="AH18" s="0" t="str">
         <v xml:space="preserve">    </v>
       </c>
       <c r="AI18" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="AJ18" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -14223,22 +14207,22 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="C19" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="D19" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="E19" s="0" t="str">
         <v xml:space="preserve">    </v>
       </c>
       <c r="F19" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="G19" s="0" t="str">
         <v xml:space="preserve">    </v>
       </c>
       <c r="H19" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="I19" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -14253,31 +14237,31 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="M19" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="N19" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="O19" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="P19" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="Q19" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="R19" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="S19" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="T19" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="U19" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="V19" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -14295,7 +14279,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AA19" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="AB19" s="0" t="str">
         <v xml:space="preserve">    </v>
@@ -14304,7 +14288,7 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="AD19" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="AE19" s="0" t="str">
         <v xml:space="preserve">    </v>
@@ -14325,13 +14309,13 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="AK19" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="AL19" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="AM19" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="AN19" s="0" t="str">
         <v xml:space="preserve">  B </v>
@@ -14348,19 +14332,19 @@
         <v xml:space="preserve">  B </v>
       </c>
       <c r="D20" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="E20" s="0" t="str">
         <v xml:space="preserve">    </v>
       </c>
       <c r="F20" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="G20" s="0" t="str">
         <v xml:space="preserve">    </v>
       </c>
       <c r="H20" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="I20" s="0" t="str">
         <v xml:space="preserve">  B </v>
@@ -14399,7 +14383,7 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="U20" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="V20" s="0" t="str">
         <v xml:space="preserve">    </v>
@@ -14417,7 +14401,7 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="AA20" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="AB20" s="0" t="str">
         <v xml:space="preserve">    </v>
@@ -14429,7 +14413,7 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="AE20" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="AF20" s="0" t="str">
         <v xml:space="preserve"> A C</v>
@@ -14438,7 +14422,7 @@
         <v xml:space="preserve">  B </v>
       </c>
       <c r="AH20" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="AI20" s="0" t="str">
         <v xml:space="preserve">    </v>
@@ -14450,7 +14434,7 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="AL20" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="AM20" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -14470,13 +14454,13 @@
         <v xml:space="preserve">  B </v>
       </c>
       <c r="D21" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="E21" s="0" t="str">
         <v xml:space="preserve">    </v>
       </c>
       <c r="F21" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="G21" s="0" t="str">
         <v xml:space="preserve">    </v>
@@ -14578,7 +14562,7 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="AN21" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
     </row>
     <row r="22" spans="1:40" customFormat="false">
@@ -14592,13 +14576,13 @@
         <v xml:space="preserve">  B </v>
       </c>
       <c r="D22" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="E22" s="0" t="str">
         <v xml:space="preserve">    </v>
       </c>
       <c r="F22" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="G22" s="0" t="str">
         <v xml:space="preserve">    </v>
@@ -14610,7 +14594,7 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="J22" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="K22" s="0" t="str">
         <v xml:space="preserve">    </v>
@@ -14667,7 +14651,7 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="AC22" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="AD22" s="0" t="str">
         <v xml:space="preserve">    </v>
@@ -14676,7 +14660,7 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="AF22" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="AG22" s="0" t="str">
         <v xml:space="preserve">    </v>
@@ -14694,7 +14678,7 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="AL22" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="AM22" s="0" t="str">
         <v xml:space="preserve">    </v>
@@ -14714,13 +14698,13 @@
         <v xml:space="preserve">  B </v>
       </c>
       <c r="D23" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="E23" s="0" t="str">
         <v xml:space="preserve">    </v>
       </c>
       <c r="F23" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="G23" s="0" t="str">
         <v xml:space="preserve">    </v>
@@ -14729,10 +14713,10 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="I23" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="J23" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="K23" s="0" t="str">
         <v xml:space="preserve">    </v>
@@ -14741,7 +14725,7 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="M23" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="N23" s="0" t="str">
         <v xml:space="preserve">    </v>
@@ -14762,13 +14746,13 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="T23" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="U23" s="0" t="str">
         <v xml:space="preserve">    </v>
       </c>
       <c r="V23" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="W23" s="0" t="str">
         <v xml:space="preserve">    </v>
@@ -14798,7 +14782,7 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="AF23" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="AG23" s="0" t="str">
         <v xml:space="preserve">  B </v>
@@ -14830,28 +14814,28 @@
         <v>INTERMEDIATE ask questions, request clarification</v>
       </c>
       <c r="B24" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="C24" s="0" t="str">
         <v xml:space="preserve">  B </v>
       </c>
       <c r="D24" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="E24" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="F24" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="G24" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="H24" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="I24" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="J24" s="0" t="str">
         <v xml:space="preserve"> A C</v>
@@ -14860,13 +14844,13 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="L24" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="M24" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="N24" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="O24" s="0" t="str">
         <v xml:space="preserve">    </v>
@@ -14884,7 +14868,7 @@
         <v xml:space="preserve">  B </v>
       </c>
       <c r="T24" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="U24" s="0" t="str">
         <v xml:space="preserve"> A C</v>
@@ -14893,7 +14877,7 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="W24" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="X24" s="0" t="str">
         <v xml:space="preserve">    </v>
@@ -14902,7 +14886,7 @@
         <v xml:space="preserve"> A C</v>
       </c>
       <c r="Z24" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="AA24" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -14923,10 +14907,10 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="AG24" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="AH24" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="AI24" s="0" t="str">
         <v xml:space="preserve">    </v>
@@ -14935,13 +14919,13 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AK24" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="AL24" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="AM24" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="AN24" s="0" t="str">
         <v xml:space="preserve">    </v>
@@ -14952,22 +14936,22 @@
         <v>INTERMEDIATE self-correct or restate when not understood</v>
       </c>
       <c r="B25" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="C25" s="0" t="str">
         <v xml:space="preserve">    </v>
       </c>
       <c r="D25" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="E25" s="0" t="str">
         <v xml:space="preserve">    </v>
       </c>
       <c r="F25" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="G25" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="H25" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -14985,19 +14969,19 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="M25" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="N25" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="O25" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="P25" s="0" t="str">
         <v xml:space="preserve">    </v>
       </c>
       <c r="Q25" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="R25" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -15021,22 +15005,22 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="Y25" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="Z25" s="0" t="str">
         <v xml:space="preserve">    </v>
       </c>
       <c r="AA25" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="AB25" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="AC25" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="AD25" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="AE25" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -15057,10 +15041,10 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AK25" s="0" t="str">
-        <v xml:space="preserve"> A C</v>
+        <v xml:space="preserve"> A  </v>
       </c>
       <c r="AL25" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="AM25" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -15125,7 +15109,7 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="S26" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="T26" s="0" t="str">
         <v xml:space="preserve">    </v>
@@ -15137,7 +15121,7 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="W26" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="X26" s="0" t="str">
         <v xml:space="preserve">  B </v>
@@ -15146,7 +15130,7 @@
         <v xml:space="preserve">    </v>
       </c>
       <c r="Z26" s="0" t="str">
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">   C</v>
       </c>
       <c r="AA26" s="0" t="str">
         <v xml:space="preserve"> ABC</v>
@@ -15164,7 +15148,7 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AF26" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="AG26" s="0" t="str">
         <v xml:space="preserve">    </v>
@@ -15182,54 +15166,16 @@
         <v xml:space="preserve"> ABC</v>
       </c>
       <c r="AL26" s="0" t="str">
-        <v xml:space="preserve">  B </v>
+        <v xml:space="preserve">  BC</v>
       </c>
       <c r="AM26" s="0" t="str">
-        <v xml:space="preserve"> ABC</v>
+        <v xml:space="preserve"> AB </v>
       </c>
       <c r="AN26" s="0" t="str">
         <v xml:space="preserve">    </v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="C2" r:id="rId2"/>
-    <hyperlink ref="D2" r:id="rId3"/>
-    <hyperlink ref="E2" r:id="rId4"/>
-    <hyperlink ref="F2" r:id="rId5"/>
-    <hyperlink ref="G2" r:id="rId6"/>
-    <hyperlink ref="H2" r:id="rId7"/>
-    <hyperlink ref="I2" r:id="rId8"/>
-    <hyperlink ref="J2" r:id="rId9"/>
-    <hyperlink ref="K2" r:id="rId10"/>
-    <hyperlink ref="L2" r:id="rId11"/>
-    <hyperlink ref="M2" r:id="rId12"/>
-    <hyperlink ref="N2" r:id="rId13"/>
-    <hyperlink ref="O2" r:id="rId14"/>
-    <hyperlink ref="Q2" r:id="rId15"/>
-    <hyperlink ref="R2" r:id="rId16"/>
-    <hyperlink ref="S2" r:id="rId17"/>
-    <hyperlink ref="U2" r:id="rId18"/>
-    <hyperlink ref="V2" r:id="rId19"/>
-    <hyperlink ref="W2" r:id="rId20"/>
-    <hyperlink ref="X2" r:id="rId21"/>
-    <hyperlink ref="Y2" r:id="rId22"/>
-    <hyperlink ref="Z2" r:id="rId23"/>
-    <hyperlink ref="AB2" r:id="rId24"/>
-    <hyperlink ref="AC2" r:id="rId25"/>
-    <hyperlink ref="AD2" r:id="rId26"/>
-    <hyperlink ref="AE2" r:id="rId27"/>
-    <hyperlink ref="AF2" r:id="rId28"/>
-    <hyperlink ref="AG2" r:id="rId29"/>
-    <hyperlink ref="AH2" r:id="rId30"/>
-    <hyperlink ref="AI2" r:id="rId31"/>
-    <hyperlink ref="AJ2" r:id="rId32"/>
-    <hyperlink ref="AK2" r:id="rId33"/>
-    <hyperlink ref="AL2" r:id="rId34"/>
-    <hyperlink ref="AM2" r:id="rId35"/>
-    <hyperlink ref="AN2" r:id="rId36"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>